<commit_message>
Added OLR wrangling, will await SQL db and some notes before test ingest
</commit_message>
<xml_diff>
--- a/galactose/OLR/OLR_galactose.xlsx
+++ b/galactose/OLR/OLR_galactose.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\galactose_network_induction\Working_Metadata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\domm-metadata\galactose\OLR\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="8820" windowHeight="4725"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="8820" windowHeight="4725" tabRatio="344"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="677">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="717">
   <si>
     <t>text</t>
   </si>
@@ -2099,21 +2099,12 @@
     <t>001</t>
   </si>
   <si>
-    <t>RawData.tar</t>
-  </si>
-  <si>
-    <t>ImageAnalysis.tar</t>
-  </si>
-  <si>
     <t>README_expNum2_RawData.txt</t>
   </si>
   <si>
     <t>Readme</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>README_expNum3_RawData.txt</t>
   </si>
   <si>
@@ -2196,6 +2187,135 @@
   </si>
   <si>
     <t>Image Analysis</t>
+  </si>
+  <si>
+    <t>2016-11-29</t>
+  </si>
+  <si>
+    <t>2015-2016</t>
+  </si>
+  <si>
+    <t>2015-01-01</t>
+  </si>
+  <si>
+    <t>2016-12-31</t>
+  </si>
+  <si>
+    <t>Stockwell, Sarah R; Rifkin, Scott A (2017): Data from: A Living Vector Field Reveals Constraints on Galactose Network Induction in Yeast. UC San Diego Library Digital Collections.</t>
+  </si>
+  <si>
+    <t>README_expNum2_ImageAnalysis.txt</t>
+  </si>
+  <si>
+    <t>README_expNum3_ImageAnalysis.txt</t>
+  </si>
+  <si>
+    <t>README_expNum4_ImageAnalysis.txt</t>
+  </si>
+  <si>
+    <t>README_expNum7_ImageAnalysis.txt</t>
+  </si>
+  <si>
+    <t>README_expNum8_ImageAnalysis.txt</t>
+  </si>
+  <si>
+    <t>README_expNum13_ImageAnalysis.txt</t>
+  </si>
+  <si>
+    <t>README_expNum16_ImageAnalysis.txt</t>
+  </si>
+  <si>
+    <t>README_expNum23_ImageAnalysis.txt</t>
+  </si>
+  <si>
+    <t>R Code</t>
+  </si>
+  <si>
+    <t>Readme - Raw Data</t>
+  </si>
+  <si>
+    <t>Readme - Image Analysis</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>README_expNum25_ImageAnalysis.txt</t>
+  </si>
+  <si>
+    <t>Sub-component</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>README_expNum24_ImageAnalysis.txt</t>
+  </si>
+  <si>
+    <t>expNum2_RawData.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum2_ImageAnalysis.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum3_RawData.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum3_ImageAnalysis.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum4_RawData.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum4_ImageAnalysis.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum7_RawData.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum7_ImageAnalysis.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum8_RawData.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum8_ImageAnalysis.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum13_RawData.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum13_ImageAnalysis.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum16_RawData.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum16_ImageAnalysis.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum23_RawData.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum23_ImageAnalysis.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum25_RawData.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum25_ImageAnalysis.tar.bz2</t>
+  </si>
+  <si>
+    <t>This package is a packrat bundle (https://rstudio.github.io/packrat/) containing everything needed to reproduce the analysis including data files and R scripts and the R libraries used at the time the analysis was done.  It should be possible to unbundle the package in R or extract it using standard unarchiving tools and run it.</t>
+  </si>
+  <si>
+    <t>expNum24_RawData.tar.bz2</t>
+  </si>
+  <si>
+    <t>expNum24_ImageAnalysis.tar.bz2</t>
+  </si>
+  <si>
+    <t>data | text</t>
   </si>
 </sst>
 </file>
@@ -2827,7 +2947,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2882,15 +3002,42 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2945,994 +3092,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="145">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC0D494"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC3D69A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFACD575"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -4243,37 +3403,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T46"/>
+  <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" style="3" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="26.5703125" style="3" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="46.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="30.28515625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="85" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.5703125" style="3" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" style="3" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="13" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="48" style="25" customWidth="1"/>
-    <col min="15" max="15" width="42.85546875" style="25" customWidth="1"/>
-    <col min="16" max="16" width="34.140625" style="25" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="34.140625" style="25" customWidth="1"/>
-    <col min="18" max="18" width="42.85546875" style="3" customWidth="1"/>
-    <col min="19" max="19" width="32.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="29.85546875" customWidth="1"/>
+    <col min="14" max="14" width="27" style="3" customWidth="1"/>
+    <col min="15" max="15" width="48" style="25" customWidth="1"/>
+    <col min="16" max="16" width="42.85546875" style="25" customWidth="1"/>
+    <col min="17" max="17" width="34.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="34.140625" style="25" customWidth="1"/>
+    <col min="19" max="19" width="42.85546875" style="3" customWidth="1"/>
+    <col min="20" max="20" width="32.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="29.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>338</v>
       </c>
@@ -4283,23 +3444,21 @@
       <c r="C1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="H1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="I1" s="16" t="s">
         <v>45</v>
-      </c>
-      <c r="I1" s="16" t="s">
-        <v>517</v>
       </c>
       <c r="J1" s="16" t="s">
         <v>450</v>
@@ -4314,1607 +3473,1908 @@
         <v>7</v>
       </c>
       <c r="N1" s="24" t="s">
+        <v>352</v>
+      </c>
+      <c r="O1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="P1" s="24" t="s">
         <v>354</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="Q1" s="24" t="s">
         <v>507</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="R1" s="24" t="s">
         <v>628</v>
       </c>
-      <c r="R1" s="16" t="s">
+      <c r="S1" s="16" t="s">
         <v>460</v>
-      </c>
-      <c r="S1" s="16" t="s">
-        <v>483</v>
       </c>
       <c r="T1" s="16" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="2" spans="1:20" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="U1" s="16" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>643</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="29" t="s">
         <v>485</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="C2" s="28"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29" t="s">
+        <v>690</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>716</v>
+      </c>
+      <c r="G2" s="28" t="s">
         <v>361</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="30" t="s">
         <v>632</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="28" t="s">
+        <v>667</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>666</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>675</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>676</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>677</v>
+      </c>
+      <c r="N2" s="28" t="s">
+        <v>678</v>
+      </c>
+      <c r="O2" s="31" t="s">
+        <v>672</v>
+      </c>
+      <c r="P2" s="32" t="s">
+        <v>671</v>
+      </c>
+      <c r="R2" s="32" t="s">
+        <v>671</v>
+      </c>
+      <c r="S2" s="28" t="s">
+        <v>668</v>
+      </c>
+      <c r="T2" s="7" t="s">
+        <v>669</v>
+      </c>
+      <c r="U2" s="7" t="s">
         <v>670</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>669</v>
-      </c>
-      <c r="N2" s="27" t="s">
-        <v>675</v>
-      </c>
-      <c r="O2" s="28" t="s">
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B3" s="29" t="s">
+        <v>693</v>
+      </c>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29" t="s">
+        <v>690</v>
+      </c>
+      <c r="F3" s="29" t="s">
+        <v>690</v>
+      </c>
+      <c r="G3" s="28"/>
+      <c r="H3" s="30" t="s">
+        <v>687</v>
+      </c>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
+      <c r="Q3" s="33" t="s">
+        <v>713</v>
+      </c>
+      <c r="R3" s="33"/>
+      <c r="S3" s="28"/>
+      <c r="T3" s="28"/>
+      <c r="U3" s="7"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B4" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>656</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F4" s="29"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="30" t="s">
+        <v>645</v>
+      </c>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="7"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>655</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F5" s="29"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="30" t="s">
+        <v>629</v>
+      </c>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="28" t="s">
         <v>674</v>
       </c>
-      <c r="Q2" s="28" t="s">
+      <c r="L5" s="28" t="s">
         <v>674</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>671</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>672</v>
-      </c>
-      <c r="T2" s="2" t="s">
+      <c r="M5" s="28" t="s">
+        <v>674</v>
+      </c>
+      <c r="N5" s="28"/>
+      <c r="O5" s="33"/>
+      <c r="P5" s="33"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="28"/>
+      <c r="T5" s="28"/>
+      <c r="U5" s="7"/>
+    </row>
+    <row r="6" spans="1:21" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>643</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>693</v>
+      </c>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="37" t="s">
+        <v>690</v>
+      </c>
+      <c r="F6" s="37"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="38" t="s">
+        <v>631</v>
+      </c>
+      <c r="I6" s="36"/>
+      <c r="J6" s="36"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="36"/>
+      <c r="M6" s="36"/>
+      <c r="N6" s="36"/>
+      <c r="O6" s="39"/>
+      <c r="P6" s="39"/>
+      <c r="Q6" s="39"/>
+      <c r="R6" s="39"/>
+      <c r="S6" s="36"/>
+      <c r="T6" s="36"/>
+      <c r="U6" s="40"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B7" s="29" t="s">
+        <v>693</v>
+      </c>
+      <c r="C7" s="28"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29" t="s">
+        <v>690</v>
+      </c>
+      <c r="F7" s="29"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="30" t="s">
+        <v>633</v>
+      </c>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="28"/>
+      <c r="M7" s="28"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="33"/>
+      <c r="P7" s="33"/>
+      <c r="Q7" s="33"/>
+      <c r="R7" s="33"/>
+      <c r="S7" s="28"/>
+      <c r="T7" s="28"/>
+      <c r="U7" s="7"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B8" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>644</v>
+      </c>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F8" s="29"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="30" t="s">
+        <v>688</v>
+      </c>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="33"/>
+      <c r="P8" s="33"/>
+      <c r="Q8" s="33"/>
+      <c r="R8" s="33"/>
+      <c r="S8" s="28"/>
+      <c r="T8" s="28"/>
+      <c r="U8" s="7"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B9" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>679</v>
+      </c>
+      <c r="D9" s="29"/>
+      <c r="E9" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F9" s="29"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="30" t="s">
+        <v>689</v>
+      </c>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="28"/>
+      <c r="M9" s="28"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="33"/>
+      <c r="P9" s="33"/>
+      <c r="Q9" s="33"/>
+      <c r="R9" s="33"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="28"/>
+      <c r="U9" s="7"/>
+    </row>
+    <row r="10" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>695</v>
+      </c>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F10" s="29"/>
+      <c r="G10" s="34"/>
+      <c r="H10" s="30" t="s">
+        <v>630</v>
+      </c>
+      <c r="I10" s="34"/>
+      <c r="J10" s="34"/>
+      <c r="K10" s="28" t="s">
+        <v>665</v>
+      </c>
+      <c r="L10" s="28" t="s">
+        <v>665</v>
+      </c>
+      <c r="M10" s="28" t="s">
+        <v>665</v>
+      </c>
+      <c r="N10" s="28"/>
+      <c r="O10" s="33"/>
+      <c r="P10" s="33"/>
+      <c r="Q10" s="33"/>
+      <c r="R10" s="33"/>
+      <c r="S10" s="34"/>
+      <c r="T10" s="34"/>
+    </row>
+    <row r="11" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>696</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F11" s="29"/>
+      <c r="G11" s="34"/>
+      <c r="H11" s="30" t="s">
         <v>673</v>
       </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="34"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
+      <c r="O11" s="33"/>
+      <c r="P11" s="33"/>
+      <c r="Q11" s="33"/>
+      <c r="R11" s="33"/>
+      <c r="S11" s="34"/>
+      <c r="T11" s="34"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A12" s="28" t="s">
         <v>643</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="G3" s="3" t="s">
+      <c r="B12" s="29" t="s">
+        <v>693</v>
+      </c>
+      <c r="C12" s="28"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29" t="s">
+        <v>690</v>
+      </c>
+      <c r="F12" s="29"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="30" t="s">
+        <v>634</v>
+      </c>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="28"/>
+      <c r="N12" s="28"/>
+      <c r="O12" s="33"/>
+      <c r="P12" s="33"/>
+      <c r="Q12" s="33"/>
+      <c r="R12" s="33"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="28"/>
+      <c r="U12" s="7"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>646</v>
+      </c>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F13" s="29"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="30" t="s">
+        <v>688</v>
+      </c>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="28"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="33"/>
+      <c r="P13" s="33"/>
+      <c r="Q13" s="33"/>
+      <c r="R13" s="33"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="7"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A14" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B14" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C14" s="28" t="s">
+        <v>680</v>
+      </c>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F14" s="29"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="30" t="s">
+        <v>689</v>
+      </c>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="28"/>
+      <c r="N14" s="28"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="33"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="28"/>
+      <c r="U14" s="7"/>
+    </row>
+    <row r="15" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B15" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>697</v>
+      </c>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F15" s="29"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="30" t="s">
+        <v>630</v>
+      </c>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="28" t="s">
+        <v>665</v>
+      </c>
+      <c r="L15" s="28" t="s">
+        <v>665</v>
+      </c>
+      <c r="M15" s="28" t="s">
+        <v>665</v>
+      </c>
+      <c r="N15" s="28"/>
+      <c r="O15" s="33"/>
+      <c r="P15" s="33"/>
+      <c r="Q15" s="33"/>
+      <c r="R15" s="33"/>
+      <c r="S15" s="34"/>
+      <c r="T15" s="34"/>
+    </row>
+    <row r="16" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B16" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>698</v>
+      </c>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F16" s="29"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="30" t="s">
+        <v>673</v>
+      </c>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34"/>
+      <c r="N16" s="34"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="34"/>
+      <c r="T16" s="34"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A17" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B17" s="29" t="s">
+        <v>693</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29" t="s">
+        <v>690</v>
+      </c>
+      <c r="F17" s="29"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="30" t="s">
+        <v>635</v>
+      </c>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="28"/>
+      <c r="U17" s="7"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B18" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>647</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F18" s="29"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="30" t="s">
+        <v>688</v>
+      </c>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="28"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="28"/>
+      <c r="N18" s="28"/>
+      <c r="O18" s="33"/>
+      <c r="P18" s="33"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="33"/>
+      <c r="S18" s="28"/>
+      <c r="T18" s="28"/>
+      <c r="U18" s="7"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B19" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>681</v>
+      </c>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F19" s="29"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="30" t="s">
+        <v>689</v>
+      </c>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="28"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="33"/>
+      <c r="R19" s="33"/>
+      <c r="S19" s="28"/>
+      <c r="T19" s="28"/>
+      <c r="U19" s="7"/>
+    </row>
+    <row r="20" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B20" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>699</v>
+      </c>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F20" s="29"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="30" t="s">
+        <v>630</v>
+      </c>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="28" t="s">
+        <v>664</v>
+      </c>
+      <c r="L20" s="28" t="s">
+        <v>664</v>
+      </c>
+      <c r="M20" s="28" t="s">
+        <v>664</v>
+      </c>
+      <c r="N20" s="28"/>
+      <c r="O20" s="33"/>
+      <c r="P20" s="33"/>
+      <c r="Q20" s="33"/>
+      <c r="R20" s="33"/>
+      <c r="S20" s="34"/>
+      <c r="T20" s="34"/>
+    </row>
+    <row r="21" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B21" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>700</v>
+      </c>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F21" s="29"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="30" t="s">
+        <v>673</v>
+      </c>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="33"/>
+      <c r="P21" s="33"/>
+      <c r="Q21" s="33"/>
+      <c r="R21" s="33"/>
+      <c r="S21" s="34"/>
+      <c r="T21" s="34"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A22" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B22" s="29" t="s">
+        <v>693</v>
+      </c>
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29" t="s">
+        <v>690</v>
+      </c>
+      <c r="F22" s="29"/>
+      <c r="G22" s="28"/>
+      <c r="H22" s="30" t="s">
+        <v>636</v>
+      </c>
+      <c r="I22" s="28"/>
+      <c r="J22" s="28"/>
+      <c r="K22" s="28"/>
+      <c r="L22" s="28"/>
+      <c r="M22" s="28"/>
+      <c r="N22" s="28"/>
+      <c r="O22" s="33"/>
+      <c r="P22" s="33"/>
+      <c r="Q22" s="33"/>
+      <c r="R22" s="33"/>
+      <c r="S22" s="28"/>
+      <c r="T22" s="28"/>
+      <c r="U22" s="7"/>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B23" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C23" s="28" t="s">
         <v>648</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B4" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="D23" s="29"/>
+      <c r="E23" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F23" s="29"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="30" t="s">
+        <v>688</v>
+      </c>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="33"/>
+      <c r="P23" s="33"/>
+      <c r="Q23" s="33"/>
+      <c r="R23" s="33"/>
+      <c r="S23" s="28"/>
+      <c r="T23" s="28"/>
+      <c r="U23" s="7"/>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B24" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>682</v>
+      </c>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F24" s="29"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="30" t="s">
+        <v>689</v>
+      </c>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33"/>
+      <c r="Q24" s="33"/>
+      <c r="R24" s="33"/>
+      <c r="S24" s="28"/>
+      <c r="T24" s="28"/>
+      <c r="U24" s="7"/>
+    </row>
+    <row r="25" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B25" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>701</v>
+      </c>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F25" s="29"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="30" t="s">
+        <v>630</v>
+      </c>
+      <c r="I25" s="34"/>
+      <c r="J25" s="34"/>
+      <c r="K25" s="28" t="s">
+        <v>663</v>
+      </c>
+      <c r="L25" s="28" t="s">
+        <v>663</v>
+      </c>
+      <c r="M25" s="28" t="s">
+        <v>663</v>
+      </c>
+      <c r="N25" s="28"/>
+      <c r="O25" s="33"/>
+      <c r="P25" s="33"/>
+      <c r="Q25" s="33"/>
+      <c r="R25" s="33"/>
+      <c r="S25" s="34"/>
+      <c r="T25" s="34"/>
+    </row>
+    <row r="26" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B26" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>702</v>
+      </c>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F26" s="29"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="30" t="s">
+        <v>673</v>
+      </c>
+      <c r="I26" s="34"/>
+      <c r="J26" s="34"/>
+      <c r="K26" s="34"/>
+      <c r="L26" s="34"/>
+      <c r="M26" s="34"/>
+      <c r="N26" s="34"/>
+      <c r="O26" s="33"/>
+      <c r="P26" s="33"/>
+      <c r="Q26" s="33"/>
+      <c r="R26" s="33"/>
+      <c r="S26" s="34"/>
+      <c r="T26" s="34"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B27" s="29" t="s">
+        <v>693</v>
+      </c>
+      <c r="C27" s="28"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29" t="s">
+        <v>690</v>
+      </c>
+      <c r="F27" s="29"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="30" t="s">
+        <v>637</v>
+      </c>
+      <c r="I27" s="28"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="33"/>
+      <c r="P27" s="33"/>
+      <c r="Q27" s="33"/>
+      <c r="R27" s="33"/>
+      <c r="S27" s="28"/>
+      <c r="T27" s="28"/>
+      <c r="U27" s="7"/>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B28" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C28" s="28" t="s">
+        <v>649</v>
+      </c>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F28" s="29"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="30" t="s">
+        <v>688</v>
+      </c>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="28"/>
+      <c r="L28" s="28"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="28"/>
+      <c r="O28" s="33"/>
+      <c r="P28" s="33"/>
+      <c r="Q28" s="33"/>
+      <c r="R28" s="33"/>
+      <c r="S28" s="28"/>
+      <c r="T28" s="28"/>
+      <c r="U28" s="7"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C29" s="28" t="s">
+        <v>683</v>
+      </c>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F29" s="29"/>
+      <c r="G29" s="28"/>
+      <c r="H29" s="30" t="s">
+        <v>689</v>
+      </c>
+      <c r="I29" s="28"/>
+      <c r="J29" s="28"/>
+      <c r="K29" s="28"/>
+      <c r="L29" s="28"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="33"/>
+      <c r="P29" s="33"/>
+      <c r="Q29" s="33"/>
+      <c r="R29" s="33"/>
+      <c r="S29" s="28"/>
+      <c r="T29" s="28"/>
+      <c r="U29" s="7"/>
+    </row>
+    <row r="30" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B30" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>703</v>
+      </c>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F30" s="29"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="30" t="s">
+        <v>630</v>
+      </c>
+      <c r="I30" s="34"/>
+      <c r="J30" s="34"/>
+      <c r="K30" s="28" t="s">
+        <v>662</v>
+      </c>
+      <c r="L30" s="28" t="s">
+        <v>662</v>
+      </c>
+      <c r="M30" s="28" t="s">
+        <v>662</v>
+      </c>
+      <c r="N30" s="28"/>
+      <c r="O30" s="33"/>
+      <c r="P30" s="33"/>
+      <c r="Q30" s="33"/>
+      <c r="R30" s="33"/>
+      <c r="S30" s="34"/>
+      <c r="T30" s="34"/>
+    </row>
+    <row r="31" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B31" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>704</v>
+      </c>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F31" s="29"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="30" t="s">
+        <v>673</v>
+      </c>
+      <c r="I31" s="34"/>
+      <c r="J31" s="34"/>
+      <c r="K31" s="34"/>
+      <c r="L31" s="34"/>
+      <c r="M31" s="34"/>
+      <c r="N31" s="34"/>
+      <c r="O31" s="33"/>
+      <c r="P31" s="33"/>
+      <c r="Q31" s="33"/>
+      <c r="R31" s="33"/>
+      <c r="S31" s="34"/>
+      <c r="T31" s="34"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B32" s="29" t="s">
+        <v>693</v>
+      </c>
+      <c r="C32" s="28"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29" t="s">
+        <v>690</v>
+      </c>
+      <c r="F32" s="29"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="30" t="s">
+        <v>638</v>
+      </c>
+      <c r="I32" s="28"/>
+      <c r="J32" s="28"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="28"/>
+      <c r="N32" s="28"/>
+      <c r="O32" s="33"/>
+      <c r="P32" s="33"/>
+      <c r="Q32" s="33"/>
+      <c r="R32" s="33"/>
+      <c r="S32" s="28"/>
+      <c r="T32" s="28"/>
+      <c r="U32" s="7"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B33" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C33" s="28" t="s">
+        <v>650</v>
+      </c>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F33" s="29"/>
+      <c r="G33" s="28"/>
+      <c r="H33" s="30" t="s">
+        <v>688</v>
+      </c>
+      <c r="I33" s="28"/>
+      <c r="J33" s="28"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="28"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="33"/>
+      <c r="P33" s="33"/>
+      <c r="Q33" s="33"/>
+      <c r="R33" s="33"/>
+      <c r="S33" s="28"/>
+      <c r="T33" s="28"/>
+      <c r="U33" s="7"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B34" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C34" s="28" t="s">
+        <v>684</v>
+      </c>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F34" s="29"/>
+      <c r="G34" s="28"/>
+      <c r="H34" s="30" t="s">
+        <v>689</v>
+      </c>
+      <c r="I34" s="28"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
+      <c r="L34" s="28"/>
+      <c r="M34" s="28"/>
+      <c r="N34" s="28"/>
+      <c r="O34" s="33"/>
+      <c r="P34" s="33"/>
+      <c r="Q34" s="33"/>
+      <c r="R34" s="33"/>
+      <c r="S34" s="28"/>
+      <c r="T34" s="28"/>
+      <c r="U34" s="7"/>
+    </row>
+    <row r="35" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B35" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>705</v>
+      </c>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F35" s="29"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="30" t="s">
+        <v>630</v>
+      </c>
+      <c r="I35" s="34"/>
+      <c r="J35" s="34"/>
+      <c r="K35" s="28" t="s">
+        <v>661</v>
+      </c>
+      <c r="L35" s="28" t="s">
+        <v>661</v>
+      </c>
+      <c r="M35" s="28" t="s">
+        <v>661</v>
+      </c>
+      <c r="N35" s="28"/>
+      <c r="O35" s="33"/>
+      <c r="P35" s="33"/>
+      <c r="Q35" s="33"/>
+      <c r="R35" s="33"/>
+      <c r="S35" s="34"/>
+      <c r="T35" s="34"/>
+    </row>
+    <row r="36" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B36" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>706</v>
+      </c>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F36" s="29"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="30" t="s">
+        <v>673</v>
+      </c>
+      <c r="I36" s="34"/>
+      <c r="J36" s="34"/>
+      <c r="K36" s="34"/>
+      <c r="L36" s="34"/>
+      <c r="M36" s="34"/>
+      <c r="N36" s="34"/>
+      <c r="O36" s="33"/>
+      <c r="P36" s="33"/>
+      <c r="Q36" s="33"/>
+      <c r="R36" s="33"/>
+      <c r="S36" s="34"/>
+      <c r="T36" s="34"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>693</v>
+      </c>
+      <c r="C37" s="28"/>
+      <c r="D37" s="29"/>
+      <c r="E37" s="29" t="s">
+        <v>690</v>
+      </c>
+      <c r="F37" s="29"/>
+      <c r="G37" s="28"/>
+      <c r="H37" s="30" t="s">
+        <v>639</v>
+      </c>
+      <c r="I37" s="28"/>
+      <c r="J37" s="28"/>
+      <c r="K37" s="28"/>
+      <c r="L37" s="28"/>
+      <c r="M37" s="28"/>
+      <c r="N37" s="28"/>
+      <c r="O37" s="33"/>
+      <c r="P37" s="33"/>
+      <c r="Q37" s="33"/>
+      <c r="R37" s="33"/>
+      <c r="S37" s="28"/>
+      <c r="T37" s="28"/>
+      <c r="U37" s="7"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C38" s="28" t="s">
+        <v>651</v>
+      </c>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F38" s="29"/>
+      <c r="G38" s="28"/>
+      <c r="H38" s="30" t="s">
+        <v>688</v>
+      </c>
+      <c r="I38" s="28"/>
+      <c r="J38" s="28"/>
+      <c r="K38" s="28"/>
+      <c r="L38" s="28"/>
+      <c r="M38" s="28"/>
+      <c r="N38" s="28"/>
+      <c r="O38" s="33"/>
+      <c r="P38" s="33"/>
+      <c r="Q38" s="33"/>
+      <c r="R38" s="33"/>
+      <c r="S38" s="28"/>
+      <c r="T38" s="28"/>
+      <c r="U38" s="7"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C39" s="28" t="s">
+        <v>685</v>
+      </c>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F39" s="29"/>
+      <c r="G39" s="28"/>
+      <c r="H39" s="30" t="s">
+        <v>689</v>
+      </c>
+      <c r="I39" s="28"/>
+      <c r="J39" s="28"/>
+      <c r="K39" s="28"/>
+      <c r="L39" s="28"/>
+      <c r="M39" s="28"/>
+      <c r="N39" s="28"/>
+      <c r="O39" s="33"/>
+      <c r="P39" s="33"/>
+      <c r="Q39" s="33"/>
+      <c r="R39" s="33"/>
+      <c r="S39" s="28"/>
+      <c r="T39" s="28"/>
+      <c r="U39" s="7"/>
+    </row>
+    <row r="40" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C40" s="34" t="s">
+        <v>707</v>
+      </c>
+      <c r="D40" s="29"/>
+      <c r="E40" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F40" s="29"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="30" t="s">
+        <v>630</v>
+      </c>
+      <c r="I40" s="34"/>
+      <c r="J40" s="34"/>
+      <c r="K40" s="28" t="s">
+        <v>660</v>
+      </c>
+      <c r="L40" s="28" t="s">
+        <v>660</v>
+      </c>
+      <c r="M40" s="28" t="s">
+        <v>660</v>
+      </c>
+      <c r="N40" s="28"/>
+      <c r="O40" s="33"/>
+      <c r="P40" s="33"/>
+      <c r="Q40" s="33"/>
+      <c r="R40" s="33"/>
+      <c r="S40" s="34"/>
+      <c r="T40" s="34"/>
+    </row>
+    <row r="41" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C41" s="34" t="s">
+        <v>708</v>
+      </c>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F41" s="29"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="30" t="s">
+        <v>673</v>
+      </c>
+      <c r="I41" s="34"/>
+      <c r="J41" s="34"/>
+      <c r="K41" s="34"/>
+      <c r="L41" s="34"/>
+      <c r="M41" s="34"/>
+      <c r="N41" s="34"/>
+      <c r="O41" s="33"/>
+      <c r="P41" s="33"/>
+      <c r="Q41" s="33"/>
+      <c r="R41" s="33"/>
+      <c r="S41" s="34"/>
+      <c r="T41" s="34"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A42" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>693</v>
+      </c>
+      <c r="C42" s="28"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29" t="s">
+        <v>690</v>
+      </c>
+      <c r="F42" s="29"/>
+      <c r="G42" s="28"/>
+      <c r="H42" s="30" t="s">
+        <v>640</v>
+      </c>
+      <c r="I42" s="28"/>
+      <c r="J42" s="28"/>
+      <c r="K42" s="28"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="28"/>
+      <c r="O42" s="33"/>
+      <c r="P42" s="33"/>
+      <c r="Q42" s="33"/>
+      <c r="R42" s="33"/>
+      <c r="S42" s="28"/>
+      <c r="T42" s="28"/>
+      <c r="U42" s="7"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B43" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C43" s="28" t="s">
+        <v>652</v>
+      </c>
+      <c r="D43" s="29"/>
+      <c r="E43" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F43" s="29"/>
+      <c r="G43" s="28"/>
+      <c r="H43" s="30" t="s">
+        <v>688</v>
+      </c>
+      <c r="I43" s="28"/>
+      <c r="J43" s="28"/>
+      <c r="K43" s="28"/>
+      <c r="L43" s="28"/>
+      <c r="M43" s="28"/>
+      <c r="N43" s="28"/>
+      <c r="O43" s="33"/>
+      <c r="P43" s="33"/>
+      <c r="Q43" s="33"/>
+      <c r="R43" s="33"/>
+      <c r="S43" s="28"/>
+      <c r="T43" s="28"/>
+      <c r="U43" s="7"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B44" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C44" s="28" t="s">
+        <v>686</v>
+      </c>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F44" s="29"/>
+      <c r="G44" s="28"/>
+      <c r="H44" s="30" t="s">
+        <v>689</v>
+      </c>
+      <c r="I44" s="28"/>
+      <c r="J44" s="28"/>
+      <c r="K44" s="28"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="28"/>
+      <c r="O44" s="33"/>
+      <c r="P44" s="33"/>
+      <c r="Q44" s="33"/>
+      <c r="R44" s="33"/>
+      <c r="S44" s="28"/>
+      <c r="T44" s="28"/>
+      <c r="U44" s="7"/>
+    </row>
+    <row r="45" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B45" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C45" s="34" t="s">
+        <v>709</v>
+      </c>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F45" s="29"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="30" t="s">
+        <v>630</v>
+      </c>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
+      <c r="K45" s="28" t="s">
         <v>659</v>
       </c>
-      <c r="G4" s="22" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="B5" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="L45" s="28" t="s">
+        <v>659</v>
+      </c>
+      <c r="M45" s="28" t="s">
+        <v>659</v>
+      </c>
+      <c r="N45" s="28"/>
+      <c r="Q45" s="33" t="s">
+        <v>657</v>
+      </c>
+      <c r="R45" s="33"/>
+      <c r="S45" s="34"/>
+      <c r="T45" s="34"/>
+    </row>
+    <row r="46" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="B46" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C46" s="34" t="s">
+        <v>710</v>
+      </c>
+      <c r="D46" s="29"/>
+      <c r="E46" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F46" s="29"/>
+      <c r="G46" s="34"/>
+      <c r="H46" s="30" t="s">
+        <v>673</v>
+      </c>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
+      <c r="K46" s="34"/>
+      <c r="L46" s="34"/>
+      <c r="M46" s="34"/>
+      <c r="N46" s="34"/>
+      <c r="O46" s="35"/>
+      <c r="P46" s="35"/>
+      <c r="Q46" s="33" t="s">
         <v>658</v>
       </c>
-      <c r="G5" s="22" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="R46" s="33"/>
+      <c r="S46" s="34"/>
+      <c r="T46" s="34"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A47" s="28" t="s">
         <v>643</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B47" s="29" t="s">
+        <v>693</v>
+      </c>
+      <c r="C47" s="28"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29" t="s">
+        <v>690</v>
+      </c>
+      <c r="F47" s="29"/>
+      <c r="G47" s="28"/>
+      <c r="H47" s="30" t="s">
+        <v>641</v>
+      </c>
+      <c r="I47" s="28"/>
+      <c r="J47" s="28"/>
+      <c r="K47" s="28"/>
+      <c r="L47" s="28"/>
+      <c r="M47" s="28"/>
+      <c r="N47" s="28"/>
+      <c r="O47" s="33"/>
+      <c r="P47" s="33"/>
+      <c r="Q47" s="33"/>
+      <c r="R47" s="33"/>
+      <c r="S47" s="28"/>
+      <c r="T47" s="28"/>
+      <c r="U47" s="7"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A48" s="28" t="s">
         <v>643</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>633</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="M7" s="3" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="B48" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>653</v>
+      </c>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F48" s="29"/>
+      <c r="G48" s="28"/>
+      <c r="H48" s="30" t="s">
+        <v>688</v>
+      </c>
+      <c r="I48" s="28"/>
+      <c r="J48" s="28"/>
+      <c r="K48" s="28"/>
+      <c r="L48" s="28"/>
+      <c r="M48" s="28"/>
+      <c r="N48" s="28"/>
+      <c r="O48" s="33"/>
+      <c r="P48" s="33"/>
+      <c r="Q48" s="33"/>
+      <c r="R48" s="33"/>
+      <c r="S48" s="28"/>
+      <c r="T48" s="28"/>
+      <c r="U48" s="7"/>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A49" s="28" t="s">
         <v>643</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>646</v>
-      </c>
-      <c r="G8" s="22" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="B49" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>694</v>
+      </c>
+      <c r="D49" s="29"/>
+      <c r="E49" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F49" s="29"/>
+      <c r="G49" s="28"/>
+      <c r="H49" s="30" t="s">
+        <v>689</v>
+      </c>
+      <c r="I49" s="28"/>
+      <c r="J49" s="28"/>
+      <c r="K49" s="28"/>
+      <c r="L49" s="28"/>
+      <c r="M49" s="28"/>
+      <c r="N49" s="28"/>
+      <c r="O49" s="33"/>
+      <c r="P49" s="33"/>
+      <c r="Q49" s="33"/>
+      <c r="R49" s="33"/>
+      <c r="S49" s="28"/>
+      <c r="T49" s="28"/>
+      <c r="U49" s="7"/>
+    </row>
+    <row r="50" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="28" t="s">
         <v>643</v>
       </c>
-      <c r="B9" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C9" s="22" t="s">
-        <v>644</v>
-      </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22" t="s">
+      <c r="B50" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>714</v>
+      </c>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F50" s="29"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="30" t="s">
         <v>630</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="22"/>
-      <c r="J9" s="22"/>
-      <c r="K9" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="M9" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="N9" s="25"/>
-      <c r="O9" s="25"/>
-      <c r="P9" s="25"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="22"/>
-      <c r="S9" s="22"/>
-    </row>
-    <row r="10" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="I50" s="34"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="28" t="s">
+        <v>659</v>
+      </c>
+      <c r="L50" s="28" t="s">
+        <v>659</v>
+      </c>
+      <c r="M50" s="28" t="s">
+        <v>659</v>
+      </c>
+      <c r="N50" s="28"/>
+      <c r="O50" s="33"/>
+      <c r="P50" s="33"/>
+      <c r="Q50" s="33"/>
+      <c r="R50" s="33"/>
+      <c r="S50" s="34"/>
+      <c r="T50" s="34"/>
+    </row>
+    <row r="51" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="28" t="s">
         <v>643</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>645</v>
-      </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22" t="s">
-        <v>676</v>
-      </c>
-      <c r="H10" s="22"/>
-      <c r="I10" s="22"/>
-      <c r="J10" s="22"/>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="22"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="22"/>
-      <c r="S10" s="22"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="B51" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>715</v>
+      </c>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F51" s="29"/>
+      <c r="G51" s="34"/>
+      <c r="H51" s="30" t="s">
+        <v>673</v>
+      </c>
+      <c r="I51" s="34"/>
+      <c r="J51" s="34"/>
+      <c r="K51" s="34"/>
+      <c r="L51" s="34"/>
+      <c r="M51" s="34"/>
+      <c r="N51" s="34"/>
+      <c r="O51" s="33"/>
+      <c r="P51" s="33"/>
+      <c r="Q51" s="33"/>
+      <c r="R51" s="33"/>
+      <c r="S51" s="34"/>
+      <c r="T51" s="34"/>
+    </row>
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A52" s="28" t="s">
         <v>643</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>634</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="M11" s="3" t="s">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="B52" s="29" t="s">
+        <v>693</v>
+      </c>
+      <c r="C52" s="28"/>
+      <c r="D52" s="29"/>
+      <c r="E52" s="29" t="s">
+        <v>690</v>
+      </c>
+      <c r="F52" s="29"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="30" t="s">
+        <v>642</v>
+      </c>
+      <c r="I52" s="28"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="28"/>
+      <c r="L52" s="28"/>
+      <c r="M52" s="28"/>
+      <c r="N52" s="28"/>
+      <c r="O52" s="33"/>
+      <c r="P52" s="33"/>
+      <c r="Q52" s="33"/>
+      <c r="R52" s="33"/>
+      <c r="S52" s="28"/>
+      <c r="T52" s="28"/>
+      <c r="U52" s="7"/>
+    </row>
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A53" s="28" t="s">
         <v>643</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>649</v>
-      </c>
-      <c r="G12" s="22" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="B53" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C53" s="28" t="s">
+        <v>654</v>
+      </c>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F53" s="29"/>
+      <c r="G53" s="28"/>
+      <c r="H53" s="30" t="s">
+        <v>688</v>
+      </c>
+      <c r="I53" s="28"/>
+      <c r="J53" s="28"/>
+      <c r="K53" s="28"/>
+      <c r="L53" s="28"/>
+      <c r="M53" s="28"/>
+      <c r="N53" s="28"/>
+      <c r="O53" s="33"/>
+      <c r="P53" s="33"/>
+      <c r="Q53" s="33"/>
+      <c r="R53" s="33"/>
+      <c r="S53" s="28"/>
+      <c r="T53" s="28"/>
+      <c r="U53" s="7"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A54" s="28" t="s">
         <v>643</v>
       </c>
-      <c r="B13" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C13" s="22" t="s">
-        <v>644</v>
-      </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22" t="s">
+      <c r="B54" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>691</v>
+      </c>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="F54" s="29"/>
+      <c r="G54" s="28"/>
+      <c r="H54" s="30" t="s">
+        <v>689</v>
+      </c>
+      <c r="I54" s="28"/>
+      <c r="J54" s="28"/>
+      <c r="K54" s="28"/>
+      <c r="L54" s="28"/>
+      <c r="M54" s="28"/>
+      <c r="N54" s="28"/>
+      <c r="O54" s="33"/>
+      <c r="P54" s="33"/>
+      <c r="Q54" s="33"/>
+      <c r="R54" s="33"/>
+      <c r="S54" s="28"/>
+      <c r="T54" s="28"/>
+      <c r="U54" s="7"/>
+    </row>
+    <row r="55" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C55" s="22" t="s">
+        <v>711</v>
+      </c>
+      <c r="D55" s="29"/>
+      <c r="E55" s="26" t="s">
+        <v>403</v>
+      </c>
+      <c r="F55" s="29"/>
+      <c r="G55" s="22"/>
+      <c r="H55" s="27" t="s">
         <v>630</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="L13" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="M13" s="3" t="s">
-        <v>668</v>
-      </c>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
-      <c r="Q13" s="25"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="22"/>
-    </row>
-    <row r="14" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="I55" s="22"/>
+      <c r="J55" s="22"/>
+      <c r="K55" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="L55" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="M55" s="3" t="s">
+        <v>659</v>
+      </c>
+      <c r="N55" s="3"/>
+      <c r="O55" s="25"/>
+      <c r="P55" s="25"/>
+      <c r="Q55" s="25"/>
+      <c r="R55" s="25"/>
+      <c r="S55" s="22"/>
+      <c r="T55" s="22"/>
+    </row>
+    <row r="56" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
         <v>643</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C14" s="22" t="s">
-        <v>645</v>
-      </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22" t="s">
-        <v>676</v>
-      </c>
-      <c r="H14" s="22"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="22"/>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="22"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="22"/>
-      <c r="S14" s="22"/>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>635</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="L15" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>667</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>650</v>
-      </c>
-      <c r="G16" s="22" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="17" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B17" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>644</v>
-      </c>
-      <c r="D17" s="22"/>
-      <c r="E17" s="22"/>
-      <c r="F17" s="22"/>
-      <c r="G17" s="22" t="s">
-        <v>630</v>
-      </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="22"/>
-      <c r="J17" s="22"/>
-      <c r="K17" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>667</v>
-      </c>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="22"/>
-      <c r="S17" s="22"/>
-    </row>
-    <row r="18" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C18" s="22" t="s">
-        <v>645</v>
-      </c>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22" t="s">
-        <v>676</v>
-      </c>
-      <c r="H18" s="22"/>
-      <c r="I18" s="22"/>
-      <c r="J18" s="22"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="22"/>
-      <c r="M18" s="22"/>
-      <c r="N18" s="25"/>
-      <c r="O18" s="25"/>
-      <c r="P18" s="25"/>
-      <c r="Q18" s="25"/>
-      <c r="R18" s="22"/>
-      <c r="S18" s="22"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>636</v>
-      </c>
-      <c r="K19" s="3" t="s">
-        <v>666</v>
-      </c>
-      <c r="L19" s="3" t="s">
-        <v>666</v>
-      </c>
-      <c r="M19" s="3" t="s">
-        <v>666</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>651</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>644</v>
-      </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22" t="s">
-        <v>630</v>
-      </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22"/>
-      <c r="J21" s="22"/>
-      <c r="K21" s="3" t="s">
-        <v>666</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>666</v>
-      </c>
-      <c r="M21" s="3" t="s">
-        <v>666</v>
-      </c>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="22"/>
-      <c r="S21" s="22"/>
-    </row>
-    <row r="22" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>645</v>
-      </c>
-      <c r="D22" s="22"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22" t="s">
-        <v>676</v>
-      </c>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22"/>
-      <c r="J22" s="22"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="22"/>
-      <c r="M22" s="22"/>
-      <c r="N22" s="25"/>
-      <c r="O22" s="25"/>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="25"/>
-      <c r="R22" s="22"/>
-      <c r="S22" s="22"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>637</v>
-      </c>
-      <c r="K23" s="3" t="s">
-        <v>665</v>
-      </c>
-      <c r="L23" s="3" t="s">
-        <v>665</v>
-      </c>
-      <c r="M23" s="3" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>652</v>
-      </c>
-      <c r="G24" s="22" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B25" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C25" s="22" t="s">
-        <v>644</v>
-      </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22" t="s">
-        <v>630</v>
-      </c>
-      <c r="H25" s="22"/>
-      <c r="I25" s="22"/>
-      <c r="J25" s="22"/>
-      <c r="K25" s="3" t="s">
-        <v>665</v>
-      </c>
-      <c r="L25" s="3" t="s">
-        <v>665</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>665</v>
-      </c>
-      <c r="N25" s="25"/>
-      <c r="O25" s="25"/>
-      <c r="P25" s="25"/>
-      <c r="Q25" s="25"/>
-      <c r="R25" s="22"/>
-      <c r="S25" s="22"/>
-    </row>
-    <row r="26" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B26" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C26" s="22" t="s">
-        <v>645</v>
-      </c>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22" t="s">
-        <v>676</v>
-      </c>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22"/>
-      <c r="J26" s="22"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="22"/>
-      <c r="M26" s="22"/>
-      <c r="N26" s="25"/>
-      <c r="O26" s="25"/>
-      <c r="P26" s="25"/>
-      <c r="Q26" s="25"/>
-      <c r="R26" s="22"/>
-      <c r="S26" s="22"/>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>638</v>
-      </c>
-      <c r="K27" s="3" t="s">
-        <v>664</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>664</v>
-      </c>
-      <c r="M27" s="3" t="s">
-        <v>664</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>653</v>
-      </c>
-      <c r="G28" s="22" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B29" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C29" s="22" t="s">
-        <v>644</v>
-      </c>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22" t="s">
-        <v>630</v>
-      </c>
-      <c r="H29" s="22"/>
-      <c r="I29" s="22"/>
-      <c r="J29" s="22"/>
-      <c r="K29" s="3" t="s">
-        <v>664</v>
-      </c>
-      <c r="L29" s="3" t="s">
-        <v>664</v>
-      </c>
-      <c r="M29" s="3" t="s">
-        <v>664</v>
-      </c>
-      <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
-      <c r="P29" s="25"/>
-      <c r="Q29" s="25"/>
-      <c r="R29" s="22"/>
-      <c r="S29" s="22"/>
-    </row>
-    <row r="30" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B30" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C30" s="22" t="s">
-        <v>645</v>
-      </c>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22" t="s">
-        <v>676</v>
-      </c>
-      <c r="H30" s="22"/>
-      <c r="I30" s="22"/>
-      <c r="J30" s="22"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="22"/>
-      <c r="M30" s="22"/>
-      <c r="N30" s="25"/>
-      <c r="O30" s="25"/>
-      <c r="P30" s="25"/>
-      <c r="Q30" s="25"/>
-      <c r="R30" s="22"/>
-      <c r="S30" s="22"/>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>639</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>663</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>663</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>654</v>
-      </c>
-      <c r="G32" s="22" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="33" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B33" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C33" s="22" t="s">
-        <v>644</v>
-      </c>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22" t="s">
-        <v>630</v>
-      </c>
-      <c r="H33" s="22"/>
-      <c r="I33" s="22"/>
-      <c r="J33" s="22"/>
-      <c r="K33" s="3" t="s">
-        <v>663</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>663</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>663</v>
-      </c>
-      <c r="N33" s="25"/>
-      <c r="O33" s="25"/>
-      <c r="P33" s="25"/>
-      <c r="Q33" s="25"/>
-      <c r="R33" s="22"/>
-      <c r="S33" s="22"/>
-    </row>
-    <row r="34" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B34" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C34" s="22" t="s">
-        <v>645</v>
-      </c>
-      <c r="D34" s="22"/>
-      <c r="E34" s="22"/>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22" t="s">
-        <v>676</v>
-      </c>
-      <c r="H34" s="22"/>
-      <c r="I34" s="22"/>
-      <c r="J34" s="22"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="22"/>
-      <c r="M34" s="22"/>
-      <c r="N34" s="25"/>
-      <c r="O34" s="25"/>
-      <c r="P34" s="25"/>
-      <c r="Q34" s="25"/>
-      <c r="R34" s="22"/>
-      <c r="S34" s="22"/>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>640</v>
-      </c>
-      <c r="K35" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="L35" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="M35" s="3" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="36" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>655</v>
-      </c>
-      <c r="G36" s="22" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="37" spans="1:19" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B37" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C37" s="22" t="s">
-        <v>644</v>
-      </c>
-      <c r="D37" s="22"/>
-      <c r="E37" s="22"/>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22" t="s">
-        <v>630</v>
-      </c>
-      <c r="H37" s="22"/>
-      <c r="I37" s="22"/>
-      <c r="J37" s="22"/>
-      <c r="K37" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="L37" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="M37" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="P37" s="25" t="s">
-        <v>660</v>
-      </c>
-      <c r="Q37" s="25"/>
-      <c r="R37" s="22"/>
-      <c r="S37" s="22"/>
-    </row>
-    <row r="38" spans="1:19" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B38" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C38" s="22" t="s">
-        <v>645</v>
-      </c>
-      <c r="D38" s="22"/>
-      <c r="E38" s="22"/>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22" t="s">
-        <v>676</v>
-      </c>
-      <c r="H38" s="22"/>
-      <c r="I38" s="22"/>
-      <c r="J38" s="22"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="22"/>
-      <c r="M38" s="22"/>
-      <c r="N38" s="26"/>
-      <c r="O38" s="26"/>
-      <c r="P38" s="25" t="s">
-        <v>661</v>
-      </c>
-      <c r="Q38" s="25"/>
-      <c r="R38" s="22"/>
-      <c r="S38" s="22"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>641</v>
-      </c>
-      <c r="K39" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="L39" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="M39" s="3" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="40" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>656</v>
-      </c>
-      <c r="G40" s="22" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="41" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B41" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C41" s="22" t="s">
-        <v>644</v>
-      </c>
-      <c r="D41" s="22"/>
-      <c r="E41" s="22"/>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22" t="s">
-        <v>630</v>
-      </c>
-      <c r="H41" s="22"/>
-      <c r="I41" s="22"/>
-      <c r="J41" s="22"/>
-      <c r="K41" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="L41" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="M41" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="N41" s="25"/>
-      <c r="O41" s="25"/>
-      <c r="P41" s="25"/>
-      <c r="Q41" s="25"/>
-      <c r="R41" s="22"/>
-      <c r="S41" s="22"/>
-    </row>
-    <row r="42" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B42" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C42" s="22" t="s">
-        <v>645</v>
-      </c>
-      <c r="D42" s="22"/>
-      <c r="E42" s="22"/>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22" t="s">
-        <v>676</v>
-      </c>
-      <c r="H42" s="22"/>
-      <c r="I42" s="22"/>
-      <c r="J42" s="22"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="22"/>
-      <c r="M42" s="22"/>
-      <c r="N42" s="25"/>
-      <c r="O42" s="25"/>
-      <c r="P42" s="25"/>
-      <c r="Q42" s="25"/>
-      <c r="R42" s="22"/>
-      <c r="S42" s="22"/>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>524</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>642</v>
-      </c>
-      <c r="K43" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="L43" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="M43" s="3" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="44" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>657</v>
-      </c>
-      <c r="G44" s="22" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="45" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B45" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C45" s="22" t="s">
-        <v>644</v>
-      </c>
-      <c r="D45" s="22"/>
-      <c r="E45" s="22"/>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22" t="s">
-        <v>630</v>
-      </c>
-      <c r="H45" s="22"/>
-      <c r="I45" s="22"/>
-      <c r="J45" s="22"/>
-      <c r="K45" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="L45" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="M45" s="3" t="s">
-        <v>662</v>
-      </c>
-      <c r="N45" s="25"/>
-      <c r="O45" s="25"/>
-      <c r="P45" s="25"/>
-      <c r="Q45" s="25"/>
-      <c r="R45" s="22"/>
-      <c r="S45" s="22"/>
-    </row>
-    <row r="46" spans="1:19" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B46" s="22" t="s">
-        <v>525</v>
-      </c>
-      <c r="C46" s="22" t="s">
-        <v>645</v>
-      </c>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22" t="s">
-        <v>676</v>
-      </c>
-      <c r="H46" s="22"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="22"/>
-      <c r="M46" s="22"/>
-      <c r="N46" s="25"/>
-      <c r="O46" s="25"/>
-      <c r="P46" s="25"/>
-      <c r="Q46" s="25"/>
-      <c r="R46" s="22"/>
-      <c r="S46" s="22"/>
+      <c r="B56" s="29" t="s">
+        <v>692</v>
+      </c>
+      <c r="C56" s="22" t="s">
+        <v>712</v>
+      </c>
+      <c r="D56" s="29"/>
+      <c r="E56" s="26" t="s">
+        <v>403</v>
+      </c>
+      <c r="F56" s="29"/>
+      <c r="G56" s="22"/>
+      <c r="H56" s="27" t="s">
+        <v>673</v>
+      </c>
+      <c r="I56" s="22"/>
+      <c r="J56" s="22"/>
+      <c r="K56" s="22"/>
+      <c r="L56" s="22"/>
+      <c r="M56" s="22"/>
+      <c r="N56" s="22"/>
+      <c r="O56" s="25"/>
+      <c r="P56" s="25"/>
+      <c r="Q56" s="25"/>
+      <c r="R56" s="25"/>
+      <c r="S56" s="22"/>
+      <c r="T56" s="22"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B47:B1048576 B1:B8">
-    <cfRule type="containsText" dxfId="144" priority="186" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="143" priority="187" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="188" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="189" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="190" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B1)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B9:B10">
-    <cfRule type="containsText" dxfId="139" priority="181" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="138" priority="182" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="137" priority="183" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="136" priority="184" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B9)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="135" priority="185" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B9)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B29:B30">
-    <cfRule type="containsText" dxfId="134" priority="86" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="133" priority="87" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="88" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="131" priority="89" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B29)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="130" priority="90" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B29)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B27">
-    <cfRule type="containsText" dxfId="129" priority="91" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="92" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="93" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="94" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B27)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="95" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B27)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B25:B26">
-    <cfRule type="containsText" dxfId="124" priority="96" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="123" priority="97" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="122" priority="98" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="99" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B25)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="100" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B25)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B23">
-    <cfRule type="containsText" dxfId="119" priority="101" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="118" priority="102" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="117" priority="103" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="104" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B23)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="105" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B23)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B21:B22">
-    <cfRule type="containsText" dxfId="114" priority="106" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="107" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="108" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="109" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B21)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="110" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B19">
-    <cfRule type="containsText" dxfId="109" priority="111" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="112" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="113" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="114" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B19)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="115" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B19)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B17:B18">
-    <cfRule type="containsText" dxfId="104" priority="116" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="103" priority="117" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="118" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="119" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B17)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="120" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B17)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B15">
-    <cfRule type="containsText" dxfId="99" priority="121" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="122" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="123" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="124" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="125" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B13:B14">
-    <cfRule type="containsText" dxfId="94" priority="126" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="127" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="128" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="129" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="130" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B11">
-    <cfRule type="containsText" dxfId="89" priority="131" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="132" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="133" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="134" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B11)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="135" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B11)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B31">
-    <cfRule type="containsText" dxfId="84" priority="81" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="83" priority="82" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="81" priority="84" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B31)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="85" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B31)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B33:B34">
-    <cfRule type="containsText" dxfId="79" priority="76" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="78" priority="77" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="77" priority="78" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="76" priority="79" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B33)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="80" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B33)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B35">
-    <cfRule type="containsText" dxfId="74" priority="71" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="72" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="72" priority="73" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="74" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B35)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="75" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B35)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B37:B38">
-    <cfRule type="containsText" dxfId="69" priority="66" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="66" priority="69" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B37)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="65" priority="70" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B37)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B39">
-    <cfRule type="containsText" dxfId="64" priority="61" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="63" priority="62" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="64" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B39)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="65" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B39)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B41:B42">
-    <cfRule type="containsText" dxfId="59" priority="56" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="57" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="59" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B41)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="55" priority="60" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B41)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B43">
-    <cfRule type="containsText" dxfId="54" priority="51" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="54" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B43)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="55" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B43)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B45:B46">
-    <cfRule type="containsText" dxfId="49" priority="46" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="47" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="48" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="49" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B45)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="50" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B45)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
-    <cfRule type="containsText" dxfId="44" priority="41" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="42" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="44" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="45" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B16">
-    <cfRule type="containsText" dxfId="39" priority="36" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="39" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="40" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B20">
-    <cfRule type="containsText" dxfId="34" priority="31" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="32" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="33" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="34" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B20)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="35" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B20)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B24">
-    <cfRule type="containsText" dxfId="29" priority="26" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="27" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="29" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B24)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="30" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B24)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B28">
-    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="22" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="24" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B28)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="25" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B28)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B32">
-    <cfRule type="containsText" dxfId="19" priority="16" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="17" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="19" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B32)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="15" priority="20" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B32)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B36">
-    <cfRule type="containsText" dxfId="14" priority="11" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="14" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B36)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B36)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B40">
-    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B40)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="10" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B40)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B44">
-    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="  \Component">
-      <formula>NOT(ISERROR(SEARCH("  \Component",B44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="Object">
-      <formula>NOT(ISERROR(SEARCH("Object",B44)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="    \Sub-component">
-      <formula>NOT(ISERROR(SEARCH("    \Sub-component",B44)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="F1"/>
+  <dataValidations count="1">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="G1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="11">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>G1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$C$1:$C$185</xm:f>
-          </x14:formula1>
-          <xm:sqref>I1</xm:sqref>
-        </x14:dataValidation>
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="9">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$D$1:$D$6</xm:f>
@@ -5925,49 +5385,49 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
-          <xm:sqref>R1</xm:sqref>
+          <xm:sqref>S1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
           </x14:formula1>
-          <xm:sqref>S1:T1</xm:sqref>
+          <xm:sqref>T1:U1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$B$1:$B$233</xm:f>
           </x14:formula1>
-          <xm:sqref>H1</xm:sqref>
+          <xm:sqref>I1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
-          <xm:sqref>N1:Q1</xm:sqref>
+          <xm:sqref>N1:R1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$B$2:$B$21</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D1048576</xm:sqref>
+          <xm:sqref>E57:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$C$2:$C$15</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
-          <x14:formula1>
-            <xm:f>'CV values'!$A$2:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>B2:B1048576</xm:sqref>
+          <xm:sqref>F57:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'CV values'!$D$2:$D$60</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>G2:G1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
+          <x14:formula1>
+            <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>H1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Wrangled CLR and OLR to prepare for test ingest
</commit_message>
<xml_diff>
--- a/galactose/OLR/OLR_galactose.xlsx
+++ b/galactose/OLR/OLR_galactose.xlsx
@@ -165,7 +165,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="959" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="710">
   <si>
     <t>text</t>
   </si>
@@ -2060,84 +2060,18 @@
     <t>Raw data</t>
   </si>
   <si>
-    <t>SQL database</t>
-  </si>
-  <si>
     <t>Data from: A Living Vector Field Reveals Constraints on Galactose Network Induction in Yeast</t>
   </si>
   <si>
-    <t>Experiment number 2</t>
-  </si>
-  <si>
-    <t>Experiment number 3</t>
-  </si>
-  <si>
-    <t>Experiment number 4</t>
-  </si>
-  <si>
-    <t>Experiment number 7</t>
-  </si>
-  <si>
-    <t>Experiment number 8</t>
-  </si>
-  <si>
-    <t>Experiment number 13</t>
-  </si>
-  <si>
-    <t>Experiment number 16</t>
-  </si>
-  <si>
-    <t>Experiment number 23</t>
-  </si>
-  <si>
-    <t>Experiment number 24</t>
-  </si>
-  <si>
-    <t>Experiment number 25</t>
-  </si>
-  <si>
     <t>001</t>
   </si>
   <si>
-    <t>README_expNum2_RawData.txt</t>
-  </si>
-  <si>
     <t>Readme</t>
   </si>
   <si>
-    <t>README_expNum3_RawData.txt</t>
-  </si>
-  <si>
-    <t>README_expNum4_RawData.txt</t>
-  </si>
-  <si>
-    <t>README_expNum7_RawData.txt</t>
-  </si>
-  <si>
-    <t>README_expNum8_RawData.txt</t>
-  </si>
-  <si>
-    <t>README_expNum13_RawData.txt</t>
-  </si>
-  <si>
-    <t>README_expNum16_RawData.txt</t>
-  </si>
-  <si>
-    <t>README_expNum23_RawData.txt</t>
-  </si>
-  <si>
-    <t>README_expNum24_RawData.txt</t>
-  </si>
-  <si>
-    <t>README_expNum25_RawData.txt</t>
-  </si>
-  <si>
     <t>RCode_YeastVectorFieldProject-2016-11-29.tar.gz</t>
   </si>
   <si>
-    <t>README.txt</t>
-  </si>
-  <si>
     <t>This data was taken on a Nikon TiE microscope in the Rifkin lab at UCSD.</t>
   </si>
   <si>
@@ -2204,54 +2138,15 @@
     <t>Stockwell, Sarah R; Rifkin, Scott A (2017): Data from: A Living Vector Field Reveals Constraints on Galactose Network Induction in Yeast. UC San Diego Library Digital Collections.</t>
   </si>
   <si>
-    <t>README_expNum2_ImageAnalysis.txt</t>
-  </si>
-  <si>
-    <t>README_expNum3_ImageAnalysis.txt</t>
-  </si>
-  <si>
-    <t>README_expNum4_ImageAnalysis.txt</t>
-  </si>
-  <si>
-    <t>README_expNum7_ImageAnalysis.txt</t>
-  </si>
-  <si>
-    <t>README_expNum8_ImageAnalysis.txt</t>
-  </si>
-  <si>
-    <t>README_expNum13_ImageAnalysis.txt</t>
-  </si>
-  <si>
-    <t>README_expNum16_ImageAnalysis.txt</t>
-  </si>
-  <si>
-    <t>README_expNum23_ImageAnalysis.txt</t>
-  </si>
-  <si>
-    <t>R Code</t>
-  </si>
-  <si>
-    <t>Readme - Raw Data</t>
-  </si>
-  <si>
-    <t>Readme - Image Analysis</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>README_expNum25_ImageAnalysis.txt</t>
-  </si>
-  <si>
     <t>Sub-component</t>
   </si>
   <si>
     <t>Component</t>
   </si>
   <si>
-    <t>README_expNum24_ImageAnalysis.txt</t>
-  </si>
-  <si>
     <t>expNum2_RawData.tar.bz2</t>
   </si>
   <si>
@@ -2316,6 +2211,90 @@
   </si>
   <si>
     <t>data | text</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>README_MatlabAndRAnalysisScripts_and_License.txt</t>
+  </si>
+  <si>
+    <t>MySQL database</t>
+  </si>
+  <si>
+    <t>README_MySQL.txt</t>
+  </si>
+  <si>
+    <t>Experiment number 2: glucose to galactose</t>
+  </si>
+  <si>
+    <t>Experiment number 3: glucose to galactose</t>
+  </si>
+  <si>
+    <t>Experiment number 13: glucose to galactose, 0.15% glucose</t>
+  </si>
+  <si>
+    <t>Experiment number 16: glucose to galactose, 0.3% glucose</t>
+  </si>
+  <si>
+    <t>Experiment number 23: glucose to galactose</t>
+  </si>
+  <si>
+    <t>Experiment number 24: glucose to galactose</t>
+  </si>
+  <si>
+    <t>Experiment number 25: glucose to galactose</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>README_expNum2.txt</t>
+  </si>
+  <si>
+    <t>StockwellRifkin_MySQLDatabase_dump.sql.bz2</t>
+  </si>
+  <si>
+    <t>README_expNum3.txt</t>
+  </si>
+  <si>
+    <t>README_expNum4.txt</t>
+  </si>
+  <si>
+    <t>README_expNum7.txt</t>
+  </si>
+  <si>
+    <t>README_expNum8.txt</t>
+  </si>
+  <si>
+    <t>README_expNum13.txt</t>
+  </si>
+  <si>
+    <t>README_expNum16.txt</t>
+  </si>
+  <si>
+    <t>README_expNum23.txt</t>
+  </si>
+  <si>
+    <t>README_expNum24.txt</t>
+  </si>
+  <si>
+    <t>README_expNum25.txt</t>
+  </si>
+  <si>
+    <t>Matlab_Code.zip</t>
+  </si>
+  <si>
+    <t>MATLAB scripts</t>
+  </si>
+  <si>
+    <t>Experiment number 4: glycerol to galactose</t>
+  </si>
+  <si>
+    <t>Experiment number 7: reinduction</t>
+  </si>
+  <si>
+    <t>Experiment number 8: glycerol to galactose</t>
   </si>
 </sst>
 </file>
@@ -2947,7 +2926,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3028,16 +3007,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="0" xfId="7" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="7"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3403,18 +3372,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U56"/>
+  <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.28515625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="51.85546875" style="3" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" style="3" customWidth="1"/>
     <col min="5" max="5" width="19.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
@@ -3499,7 +3468,7 @@
     </row>
     <row r="2" spans="1:21" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B2" s="29" t="s">
         <v>485</v>
@@ -3507,72 +3476,72 @@
       <c r="C2" s="28"/>
       <c r="D2" s="29"/>
       <c r="E2" s="29" t="s">
-        <v>690</v>
+        <v>657</v>
       </c>
       <c r="F2" s="29" t="s">
-        <v>716</v>
+        <v>681</v>
       </c>
       <c r="G2" s="28" t="s">
         <v>361</v>
       </c>
       <c r="H2" s="30" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>667</v>
+        <v>645</v>
       </c>
       <c r="J2" s="28" t="s">
-        <v>666</v>
+        <v>644</v>
       </c>
       <c r="K2" s="28" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="L2" s="28" t="s">
-        <v>676</v>
+        <v>654</v>
       </c>
       <c r="M2" s="28" t="s">
-        <v>677</v>
+        <v>655</v>
       </c>
       <c r="N2" s="28" t="s">
-        <v>678</v>
+        <v>656</v>
       </c>
       <c r="O2" s="31" t="s">
-        <v>672</v>
+        <v>650</v>
       </c>
       <c r="P2" s="32" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="R2" s="32" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
       <c r="S2" s="28" t="s">
-        <v>668</v>
+        <v>646</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>669</v>
+        <v>647</v>
       </c>
       <c r="U2" s="7" t="s">
-        <v>670</v>
+        <v>648</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B3" s="29" t="s">
-        <v>693</v>
+        <v>659</v>
       </c>
       <c r="C3" s="28"/>
       <c r="D3" s="29"/>
       <c r="E3" s="29" t="s">
-        <v>690</v>
+        <v>657</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>690</v>
+        <v>657</v>
       </c>
       <c r="G3" s="28"/>
       <c r="H3" s="30" t="s">
-        <v>687</v>
+        <v>682</v>
       </c>
       <c r="I3" s="28"/>
       <c r="J3" s="28"/>
@@ -3583,7 +3552,7 @@
       <c r="O3" s="33"/>
       <c r="P3" s="33"/>
       <c r="Q3" s="33" t="s">
-        <v>713</v>
+        <v>678</v>
       </c>
       <c r="R3" s="33"/>
       <c r="S3" s="28"/>
@@ -3592,13 +3561,13 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B4" s="29" t="s">
-        <v>692</v>
+        <v>658</v>
       </c>
       <c r="C4" s="28" t="s">
-        <v>656</v>
+        <v>683</v>
       </c>
       <c r="D4" s="29"/>
       <c r="E4" s="29" t="s">
@@ -3607,7 +3576,7 @@
       <c r="F4" s="29"/>
       <c r="G4" s="28"/>
       <c r="H4" s="30" t="s">
-        <v>645</v>
+        <v>633</v>
       </c>
       <c r="I4" s="28"/>
       <c r="J4" s="28"/>
@@ -3625,13 +3594,13 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>655</v>
+        <v>658</v>
+      </c>
+      <c r="C5" t="s">
+        <v>705</v>
       </c>
       <c r="D5" s="29"/>
       <c r="E5" s="29" t="s">
@@ -3640,19 +3609,13 @@
       <c r="F5" s="29"/>
       <c r="G5" s="28"/>
       <c r="H5" s="30" t="s">
-        <v>629</v>
+        <v>706</v>
       </c>
       <c r="I5" s="28"/>
       <c r="J5" s="28"/>
-      <c r="K5" s="28" t="s">
-        <v>674</v>
-      </c>
-      <c r="L5" s="28" t="s">
-        <v>674</v>
-      </c>
-      <c r="M5" s="28" t="s">
-        <v>674</v>
-      </c>
+      <c r="K5" s="28"/>
+      <c r="L5" s="28"/>
+      <c r="M5" s="28"/>
       <c r="N5" s="28"/>
       <c r="O5" s="33"/>
       <c r="P5" s="33"/>
@@ -3662,286 +3625,285 @@
       <c r="T5" s="28"/>
       <c r="U5" s="7"/>
     </row>
-    <row r="6" spans="1:21" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
-        <v>643</v>
-      </c>
-      <c r="B6" s="37" t="s">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="28" t="s">
+        <v>632</v>
+      </c>
+      <c r="B6" s="29" t="s">
+        <v>658</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>634</v>
+      </c>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29" t="s">
+        <v>403</v>
+      </c>
+      <c r="F6" s="29"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="30" t="s">
+        <v>629</v>
+      </c>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="28" t="s">
+        <v>652</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>652</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>652</v>
+      </c>
+      <c r="N6" s="28"/>
+      <c r="O6" s="33"/>
+      <c r="P6" s="33"/>
+      <c r="Q6" s="33"/>
+      <c r="R6" s="33"/>
+      <c r="S6" s="28"/>
+      <c r="T6" s="28"/>
+      <c r="U6" s="7"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>632</v>
+      </c>
+      <c r="B7" t="s">
+        <v>659</v>
+      </c>
+      <c r="D7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7" t="s">
+        <v>684</v>
+      </c>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>632</v>
+      </c>
+      <c r="B8" t="s">
+        <v>658</v>
+      </c>
+      <c r="C8" t="s">
+        <v>685</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8" t="s">
+        <v>384</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8" t="s">
+        <v>633</v>
+      </c>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>632</v>
+      </c>
+      <c r="B9" t="s">
+        <v>658</v>
+      </c>
+      <c r="C9" t="s">
+        <v>695</v>
+      </c>
+      <c r="D9"/>
+      <c r="E9" t="s">
+        <v>403</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9" t="s">
         <v>693</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="37" t="s">
-        <v>690</v>
-      </c>
-      <c r="F6" s="37"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="38" t="s">
-        <v>631</v>
-      </c>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="39"/>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="36"/>
-      <c r="T6" s="36"/>
-      <c r="U6" s="40"/>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="28" t="s">
-        <v>643</v>
-      </c>
-      <c r="B7" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29" t="s">
-        <v>690</v>
-      </c>
-      <c r="F7" s="29"/>
-      <c r="G7" s="28"/>
-      <c r="H7" s="30" t="s">
-        <v>633</v>
-      </c>
-      <c r="I7" s="28"/>
-      <c r="J7" s="28"/>
-      <c r="K7" s="28"/>
-      <c r="L7" s="28"/>
-      <c r="M7" s="28"/>
-      <c r="N7" s="28"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
-      <c r="S7" s="28"/>
-      <c r="T7" s="28"/>
-      <c r="U7" s="7"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
-        <v>643</v>
-      </c>
-      <c r="B8" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>644</v>
-      </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29" t="s">
-        <v>384</v>
-      </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="30" t="s">
-        <v>688</v>
-      </c>
-      <c r="I8" s="28"/>
-      <c r="J8" s="28"/>
-      <c r="K8" s="28"/>
-      <c r="L8" s="28"/>
-      <c r="M8" s="28"/>
-      <c r="N8" s="28"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="33"/>
-      <c r="S8" s="28"/>
-      <c r="T8" s="28"/>
-      <c r="U8" s="7"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="28" t="s">
-        <v>643</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C9" s="28" t="s">
-        <v>679</v>
-      </c>
-      <c r="D9" s="29"/>
-      <c r="E9" s="29" t="s">
-        <v>384</v>
-      </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="30" t="s">
-        <v>689</v>
-      </c>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="28"/>
-      <c r="N9" s="28"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="33"/>
-      <c r="S9" s="28"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="7"/>
-    </row>
-    <row r="10" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C10" s="34" t="s">
-        <v>695</v>
-      </c>
+        <v>659</v>
+      </c>
+      <c r="C10" s="28"/>
       <c r="D10" s="29"/>
       <c r="E10" s="29" t="s">
-        <v>403</v>
+        <v>657</v>
       </c>
       <c r="F10" s="29"/>
-      <c r="G10" s="34"/>
+      <c r="G10" s="28"/>
       <c r="H10" s="30" t="s">
-        <v>630</v>
-      </c>
-      <c r="I10" s="34"/>
-      <c r="J10" s="34"/>
-      <c r="K10" s="28" t="s">
-        <v>665</v>
-      </c>
-      <c r="L10" s="28" t="s">
-        <v>665</v>
-      </c>
-      <c r="M10" s="28" t="s">
-        <v>665</v>
-      </c>
+        <v>686</v>
+      </c>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
       <c r="N10" s="28"/>
       <c r="O10" s="33"/>
       <c r="P10" s="33"/>
       <c r="Q10" s="33"/>
       <c r="R10" s="33"/>
-      <c r="S10" s="34"/>
-      <c r="T10" s="34"/>
-    </row>
-    <row r="11" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S10" s="28"/>
+      <c r="T10" s="28"/>
+      <c r="U10" s="7"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C11" s="34" t="s">
-        <v>696</v>
+        <v>658</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>694</v>
       </c>
       <c r="D11" s="29"/>
       <c r="E11" s="29" t="s">
-        <v>403</v>
+        <v>384</v>
       </c>
       <c r="F11" s="29"/>
-      <c r="G11" s="34"/>
+      <c r="G11" s="28"/>
       <c r="H11" s="30" t="s">
-        <v>673</v>
-      </c>
-      <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
+        <v>633</v>
+      </c>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
       <c r="O11" s="33"/>
       <c r="P11" s="33"/>
       <c r="Q11" s="33"/>
       <c r="R11" s="33"/>
-      <c r="S11" s="34"/>
-      <c r="T11" s="34"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S11" s="28"/>
+      <c r="T11" s="28"/>
+      <c r="U11" s="7"/>
+    </row>
+    <row r="12" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="C12" s="28"/>
+        <v>658</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>660</v>
+      </c>
       <c r="D12" s="29"/>
       <c r="E12" s="29" t="s">
-        <v>690</v>
+        <v>403</v>
       </c>
       <c r="F12" s="29"/>
-      <c r="G12" s="28"/>
+      <c r="G12" s="34"/>
       <c r="H12" s="30" t="s">
-        <v>634</v>
-      </c>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="28"/>
+        <v>630</v>
+      </c>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="L12" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="M12" s="28" t="s">
+        <v>643</v>
+      </c>
       <c r="N12" s="28"/>
       <c r="O12" s="33"/>
       <c r="P12" s="33"/>
       <c r="Q12" s="33"/>
       <c r="R12" s="33"/>
-      <c r="S12" s="28"/>
-      <c r="T12" s="28"/>
-      <c r="U12" s="7"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S12" s="34"/>
+      <c r="T12" s="34"/>
+    </row>
+    <row r="13" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>646</v>
+        <v>658</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>661</v>
       </c>
       <c r="D13" s="29"/>
       <c r="E13" s="29" t="s">
-        <v>384</v>
+        <v>403</v>
       </c>
       <c r="F13" s="29"/>
-      <c r="G13" s="28"/>
+      <c r="G13" s="34"/>
       <c r="H13" s="30" t="s">
-        <v>688</v>
-      </c>
-      <c r="I13" s="28"/>
-      <c r="J13" s="28"/>
-      <c r="K13" s="28"/>
-      <c r="L13" s="28"/>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
+        <v>651</v>
+      </c>
+      <c r="I13" s="34"/>
+      <c r="J13" s="34"/>
+      <c r="K13" s="34"/>
+      <c r="L13" s="34"/>
+      <c r="M13" s="34"/>
+      <c r="N13" s="34"/>
       <c r="O13" s="33"/>
       <c r="P13" s="33"/>
       <c r="Q13" s="33"/>
       <c r="R13" s="33"/>
-      <c r="S13" s="28"/>
-      <c r="T13" s="28"/>
-      <c r="U13" s="7"/>
+      <c r="S13" s="34"/>
+      <c r="T13" s="34"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C14" s="28" t="s">
-        <v>680</v>
-      </c>
+        <v>659</v>
+      </c>
+      <c r="C14" s="28"/>
       <c r="D14" s="29"/>
       <c r="E14" s="29" t="s">
-        <v>384</v>
+        <v>657</v>
       </c>
       <c r="F14" s="29"/>
       <c r="G14" s="28"/>
       <c r="H14" s="30" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="I14" s="28"/>
       <c r="J14" s="28"/>
@@ -3957,53 +3919,48 @@
       <c r="T14" s="28"/>
       <c r="U14" s="7"/>
     </row>
-    <row r="15" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C15" s="34" t="s">
-        <v>697</v>
+        <v>658</v>
+      </c>
+      <c r="C15" s="28" t="s">
+        <v>696</v>
       </c>
       <c r="D15" s="29"/>
       <c r="E15" s="29" t="s">
-        <v>403</v>
+        <v>384</v>
       </c>
       <c r="F15" s="29"/>
-      <c r="G15" s="34"/>
+      <c r="G15" s="28"/>
       <c r="H15" s="30" t="s">
-        <v>630</v>
-      </c>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="28" t="s">
-        <v>665</v>
-      </c>
-      <c r="L15" s="28" t="s">
-        <v>665</v>
-      </c>
-      <c r="M15" s="28" t="s">
-        <v>665</v>
-      </c>
+        <v>633</v>
+      </c>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="28"/>
       <c r="N15" s="28"/>
       <c r="O15" s="33"/>
       <c r="P15" s="33"/>
       <c r="Q15" s="33"/>
       <c r="R15" s="33"/>
-      <c r="S15" s="34"/>
-      <c r="T15" s="34"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="28"/>
+      <c r="U15" s="7"/>
     </row>
     <row r="16" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>692</v>
+        <v>658</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>698</v>
+        <v>662</v>
       </c>
       <c r="D16" s="29"/>
       <c r="E16" s="29" t="s">
@@ -4012,14 +3969,20 @@
       <c r="F16" s="29"/>
       <c r="G16" s="34"/>
       <c r="H16" s="30" t="s">
-        <v>673</v>
+        <v>630</v>
       </c>
       <c r="I16" s="34"/>
       <c r="J16" s="34"/>
-      <c r="K16" s="34"/>
-      <c r="L16" s="34"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
+      <c r="K16" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="L16" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="M16" s="28" t="s">
+        <v>643</v>
+      </c>
+      <c r="N16" s="28"/>
       <c r="O16" s="33"/>
       <c r="P16" s="33"/>
       <c r="Q16" s="33"/>
@@ -4027,55 +3990,54 @@
       <c r="S16" s="34"/>
       <c r="T16" s="34"/>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="C17" s="28"/>
+        <v>658</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>663</v>
+      </c>
       <c r="D17" s="29"/>
       <c r="E17" s="29" t="s">
-        <v>690</v>
+        <v>403</v>
       </c>
       <c r="F17" s="29"/>
-      <c r="G17" s="28"/>
+      <c r="G17" s="34"/>
       <c r="H17" s="30" t="s">
-        <v>635</v>
-      </c>
-      <c r="I17" s="28"/>
-      <c r="J17" s="28"/>
-      <c r="K17" s="28"/>
-      <c r="L17" s="28"/>
-      <c r="M17" s="28"/>
-      <c r="N17" s="28"/>
+        <v>651</v>
+      </c>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
       <c r="O17" s="33"/>
       <c r="P17" s="33"/>
       <c r="Q17" s="33"/>
       <c r="R17" s="33"/>
-      <c r="S17" s="28"/>
-      <c r="T17" s="28"/>
-      <c r="U17" s="7"/>
+      <c r="S17" s="34"/>
+      <c r="T17" s="34"/>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C18" s="28" t="s">
-        <v>647</v>
-      </c>
+        <v>659</v>
+      </c>
+      <c r="C18" s="28"/>
       <c r="D18" s="29"/>
       <c r="E18" s="29" t="s">
-        <v>384</v>
+        <v>657</v>
       </c>
       <c r="F18" s="29"/>
       <c r="G18" s="28"/>
       <c r="H18" s="30" t="s">
-        <v>688</v>
+        <v>707</v>
       </c>
       <c r="I18" s="28"/>
       <c r="J18" s="28"/>
@@ -4093,13 +4055,13 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>692</v>
+        <v>658</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>681</v>
+        <v>697</v>
       </c>
       <c r="D19" s="29"/>
       <c r="E19" s="29" t="s">
@@ -4108,7 +4070,7 @@
       <c r="F19" s="29"/>
       <c r="G19" s="28"/>
       <c r="H19" s="30" t="s">
-        <v>689</v>
+        <v>633</v>
       </c>
       <c r="I19" s="28"/>
       <c r="J19" s="28"/>
@@ -4126,13 +4088,13 @@
     </row>
     <row r="20" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>692</v>
+        <v>658</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>699</v>
+        <v>664</v>
       </c>
       <c r="D20" s="29"/>
       <c r="E20" s="29" t="s">
@@ -4146,13 +4108,13 @@
       <c r="I20" s="34"/>
       <c r="J20" s="34"/>
       <c r="K20" s="28" t="s">
-        <v>664</v>
+        <v>642</v>
       </c>
       <c r="L20" s="28" t="s">
-        <v>664</v>
+        <v>642</v>
       </c>
       <c r="M20" s="28" t="s">
-        <v>664</v>
+        <v>642</v>
       </c>
       <c r="N20" s="28"/>
       <c r="O20" s="33"/>
@@ -4164,13 +4126,13 @@
     </row>
     <row r="21" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>692</v>
+        <v>658</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>700</v>
+        <v>665</v>
       </c>
       <c r="D21" s="29"/>
       <c r="E21" s="29" t="s">
@@ -4179,7 +4141,7 @@
       <c r="F21" s="29"/>
       <c r="G21" s="34"/>
       <c r="H21" s="30" t="s">
-        <v>673</v>
+        <v>651</v>
       </c>
       <c r="I21" s="34"/>
       <c r="J21" s="34"/>
@@ -4196,20 +4158,20 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B22" s="29" t="s">
-        <v>693</v>
+        <v>659</v>
       </c>
       <c r="C22" s="28"/>
       <c r="D22" s="29"/>
       <c r="E22" s="29" t="s">
-        <v>690</v>
+        <v>657</v>
       </c>
       <c r="F22" s="29"/>
       <c r="G22" s="28"/>
       <c r="H22" s="30" t="s">
-        <v>636</v>
+        <v>708</v>
       </c>
       <c r="I22" s="28"/>
       <c r="J22" s="28"/>
@@ -4227,13 +4189,13 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>692</v>
+        <v>658</v>
       </c>
       <c r="C23" s="28" t="s">
-        <v>648</v>
+        <v>698</v>
       </c>
       <c r="D23" s="29"/>
       <c r="E23" s="29" t="s">
@@ -4242,7 +4204,7 @@
       <c r="F23" s="29"/>
       <c r="G23" s="28"/>
       <c r="H23" s="30" t="s">
-        <v>688</v>
+        <v>633</v>
       </c>
       <c r="I23" s="28"/>
       <c r="J23" s="28"/>
@@ -4258,48 +4220,53 @@
       <c r="T23" s="28"/>
       <c r="U23" s="7"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>682</v>
+        <v>658</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>666</v>
       </c>
       <c r="D24" s="29"/>
       <c r="E24" s="29" t="s">
-        <v>384</v>
+        <v>403</v>
       </c>
       <c r="F24" s="29"/>
-      <c r="G24" s="28"/>
+      <c r="G24" s="34"/>
       <c r="H24" s="30" t="s">
-        <v>689</v>
-      </c>
-      <c r="I24" s="28"/>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="M24" s="28"/>
+        <v>630</v>
+      </c>
+      <c r="I24" s="34"/>
+      <c r="J24" s="34"/>
+      <c r="K24" s="28" t="s">
+        <v>641</v>
+      </c>
+      <c r="L24" s="28" t="s">
+        <v>641</v>
+      </c>
+      <c r="M24" s="28" t="s">
+        <v>641</v>
+      </c>
       <c r="N24" s="28"/>
       <c r="O24" s="33"/>
       <c r="P24" s="33"/>
       <c r="Q24" s="33"/>
       <c r="R24" s="33"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="28"/>
-      <c r="U24" s="7"/>
+      <c r="S24" s="34"/>
+      <c r="T24" s="34"/>
     </row>
     <row r="25" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>692</v>
+        <v>658</v>
       </c>
       <c r="C25" s="34" t="s">
-        <v>701</v>
+        <v>667</v>
       </c>
       <c r="D25" s="29"/>
       <c r="E25" s="29" t="s">
@@ -4308,20 +4275,14 @@
       <c r="F25" s="29"/>
       <c r="G25" s="34"/>
       <c r="H25" s="30" t="s">
-        <v>630</v>
+        <v>651</v>
       </c>
       <c r="I25" s="34"/>
       <c r="J25" s="34"/>
-      <c r="K25" s="28" t="s">
-        <v>663</v>
-      </c>
-      <c r="L25" s="28" t="s">
-        <v>663</v>
-      </c>
-      <c r="M25" s="28" t="s">
-        <v>663</v>
-      </c>
-      <c r="N25" s="28"/>
+      <c r="K25" s="34"/>
+      <c r="L25" s="34"/>
+      <c r="M25" s="34"/>
+      <c r="N25" s="34"/>
       <c r="O25" s="33"/>
       <c r="P25" s="33"/>
       <c r="Q25" s="33"/>
@@ -4329,54 +4290,55 @@
       <c r="S25" s="34"/>
       <c r="T25" s="34"/>
     </row>
-    <row r="26" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C26" s="34" t="s">
-        <v>702</v>
-      </c>
+        <v>659</v>
+      </c>
+      <c r="C26" s="28"/>
       <c r="D26" s="29"/>
       <c r="E26" s="29" t="s">
-        <v>403</v>
+        <v>657</v>
       </c>
       <c r="F26" s="29"/>
-      <c r="G26" s="34"/>
+      <c r="G26" s="28"/>
       <c r="H26" s="30" t="s">
-        <v>673</v>
-      </c>
-      <c r="I26" s="34"/>
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
+        <v>709</v>
+      </c>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
       <c r="O26" s="33"/>
       <c r="P26" s="33"/>
       <c r="Q26" s="33"/>
       <c r="R26" s="33"/>
-      <c r="S26" s="34"/>
-      <c r="T26" s="34"/>
+      <c r="S26" s="28"/>
+      <c r="T26" s="28"/>
+      <c r="U26" s="7"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="C27" s="28"/>
+        <v>658</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>699</v>
+      </c>
       <c r="D27" s="29"/>
       <c r="E27" s="29" t="s">
-        <v>690</v>
+        <v>384</v>
       </c>
       <c r="F27" s="29"/>
       <c r="G27" s="28"/>
       <c r="H27" s="30" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="I27" s="28"/>
       <c r="J27" s="28"/>
@@ -4392,219 +4354,221 @@
       <c r="T27" s="28"/>
       <c r="U27" s="7"/>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C28" s="28" t="s">
-        <v>649</v>
+        <v>658</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>668</v>
       </c>
       <c r="D28" s="29"/>
       <c r="E28" s="29" t="s">
-        <v>384</v>
+        <v>403</v>
       </c>
       <c r="F28" s="29"/>
-      <c r="G28" s="28"/>
+      <c r="G28" s="34"/>
       <c r="H28" s="30" t="s">
-        <v>688</v>
-      </c>
-      <c r="I28" s="28"/>
-      <c r="J28" s="28"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="28"/>
+        <v>630</v>
+      </c>
+      <c r="I28" s="34"/>
+      <c r="J28" s="34"/>
+      <c r="K28" s="28" t="s">
+        <v>640</v>
+      </c>
+      <c r="L28" s="28" t="s">
+        <v>640</v>
+      </c>
+      <c r="M28" s="28" t="s">
+        <v>640</v>
+      </c>
       <c r="N28" s="28"/>
       <c r="O28" s="33"/>
       <c r="P28" s="33"/>
       <c r="Q28" s="33"/>
       <c r="R28" s="33"/>
-      <c r="S28" s="28"/>
-      <c r="T28" s="28"/>
-      <c r="U28" s="7"/>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S28" s="34"/>
+      <c r="T28" s="34"/>
+    </row>
+    <row r="29" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C29" s="28" t="s">
-        <v>683</v>
+        <v>658</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>669</v>
       </c>
       <c r="D29" s="29"/>
       <c r="E29" s="29" t="s">
-        <v>384</v>
+        <v>403</v>
       </c>
       <c r="F29" s="29"/>
-      <c r="G29" s="28"/>
+      <c r="G29" s="34"/>
       <c r="H29" s="30" t="s">
-        <v>689</v>
-      </c>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
+        <v>651</v>
+      </c>
+      <c r="I29" s="34"/>
+      <c r="J29" s="34"/>
+      <c r="K29" s="34"/>
+      <c r="L29" s="34"/>
+      <c r="M29" s="34"/>
+      <c r="N29" s="34"/>
       <c r="O29" s="33"/>
       <c r="P29" s="33"/>
       <c r="Q29" s="33"/>
       <c r="R29" s="33"/>
-      <c r="S29" s="28"/>
-      <c r="T29" s="28"/>
-      <c r="U29" s="7"/>
-    </row>
-    <row r="30" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S29" s="34"/>
+      <c r="T29" s="34"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C30" s="34" t="s">
-        <v>703</v>
-      </c>
+        <v>659</v>
+      </c>
+      <c r="C30" s="28"/>
       <c r="D30" s="29"/>
       <c r="E30" s="29" t="s">
-        <v>403</v>
+        <v>657</v>
       </c>
       <c r="F30" s="29"/>
-      <c r="G30" s="34"/>
+      <c r="G30" s="28"/>
       <c r="H30" s="30" t="s">
-        <v>630</v>
-      </c>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="28" t="s">
-        <v>662</v>
-      </c>
-      <c r="L30" s="28" t="s">
-        <v>662</v>
-      </c>
-      <c r="M30" s="28" t="s">
-        <v>662</v>
-      </c>
+        <v>688</v>
+      </c>
+      <c r="I30" s="28"/>
+      <c r="J30" s="28"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="28"/>
       <c r="N30" s="28"/>
       <c r="O30" s="33"/>
       <c r="P30" s="33"/>
       <c r="Q30" s="33"/>
       <c r="R30" s="33"/>
-      <c r="S30" s="34"/>
-      <c r="T30" s="34"/>
-    </row>
-    <row r="31" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="S30" s="28"/>
+      <c r="T30" s="28"/>
+      <c r="U30" s="7"/>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B31" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C31" s="34" t="s">
-        <v>704</v>
+        <v>658</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>700</v>
       </c>
       <c r="D31" s="29"/>
       <c r="E31" s="29" t="s">
-        <v>403</v>
+        <v>384</v>
       </c>
       <c r="F31" s="29"/>
-      <c r="G31" s="34"/>
+      <c r="G31" s="28"/>
       <c r="H31" s="30" t="s">
-        <v>673</v>
-      </c>
-      <c r="I31" s="34"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="34"/>
-      <c r="L31" s="34"/>
-      <c r="M31" s="34"/>
-      <c r="N31" s="34"/>
+        <v>633</v>
+      </c>
+      <c r="I31" s="28"/>
+      <c r="J31" s="28"/>
+      <c r="K31" s="28"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="28"/>
+      <c r="N31" s="28"/>
       <c r="O31" s="33"/>
       <c r="P31" s="33"/>
       <c r="Q31" s="33"/>
       <c r="R31" s="33"/>
-      <c r="S31" s="34"/>
-      <c r="T31" s="34"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S31" s="28"/>
+      <c r="T31" s="28"/>
+      <c r="U31" s="7"/>
+    </row>
+    <row r="32" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="C32" s="28"/>
+        <v>658</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>670</v>
+      </c>
       <c r="D32" s="29"/>
       <c r="E32" s="29" t="s">
-        <v>690</v>
+        <v>403</v>
       </c>
       <c r="F32" s="29"/>
-      <c r="G32" s="28"/>
+      <c r="G32" s="34"/>
       <c r="H32" s="30" t="s">
-        <v>638</v>
-      </c>
-      <c r="I32" s="28"/>
-      <c r="J32" s="28"/>
-      <c r="K32" s="28"/>
-      <c r="L32" s="28"/>
-      <c r="M32" s="28"/>
+        <v>630</v>
+      </c>
+      <c r="I32" s="34"/>
+      <c r="J32" s="34"/>
+      <c r="K32" s="28" t="s">
+        <v>639</v>
+      </c>
+      <c r="L32" s="28" t="s">
+        <v>639</v>
+      </c>
+      <c r="M32" s="28" t="s">
+        <v>639</v>
+      </c>
       <c r="N32" s="28"/>
       <c r="O32" s="33"/>
       <c r="P32" s="33"/>
       <c r="Q32" s="33"/>
       <c r="R32" s="33"/>
-      <c r="S32" s="28"/>
-      <c r="T32" s="28"/>
-      <c r="U32" s="7"/>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S32" s="34"/>
+      <c r="T32" s="34"/>
+    </row>
+    <row r="33" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C33" s="28" t="s">
-        <v>650</v>
+        <v>658</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>671</v>
       </c>
       <c r="D33" s="29"/>
       <c r="E33" s="29" t="s">
-        <v>384</v>
+        <v>403</v>
       </c>
       <c r="F33" s="29"/>
-      <c r="G33" s="28"/>
+      <c r="G33" s="34"/>
       <c r="H33" s="30" t="s">
-        <v>688</v>
-      </c>
-      <c r="I33" s="28"/>
-      <c r="J33" s="28"/>
-      <c r="K33" s="28"/>
-      <c r="L33" s="28"/>
-      <c r="M33" s="28"/>
-      <c r="N33" s="28"/>
+        <v>651</v>
+      </c>
+      <c r="I33" s="34"/>
+      <c r="J33" s="34"/>
+      <c r="K33" s="34"/>
+      <c r="L33" s="34"/>
+      <c r="M33" s="34"/>
+      <c r="N33" s="34"/>
       <c r="O33" s="33"/>
       <c r="P33" s="33"/>
       <c r="Q33" s="33"/>
       <c r="R33" s="33"/>
-      <c r="S33" s="28"/>
-      <c r="T33" s="28"/>
-      <c r="U33" s="7"/>
+      <c r="S33" s="34"/>
+      <c r="T33" s="34"/>
     </row>
     <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C34" s="28" t="s">
-        <v>684</v>
-      </c>
+        <v>659</v>
+      </c>
+      <c r="C34" s="28"/>
       <c r="D34" s="29"/>
       <c r="E34" s="29" t="s">
-        <v>384</v>
+        <v>657</v>
       </c>
       <c r="F34" s="29"/>
       <c r="G34" s="28"/>
@@ -4625,53 +4589,48 @@
       <c r="T34" s="28"/>
       <c r="U34" s="7"/>
     </row>
-    <row r="35" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C35" s="34" t="s">
-        <v>705</v>
+        <v>658</v>
+      </c>
+      <c r="C35" s="28" t="s">
+        <v>701</v>
       </c>
       <c r="D35" s="29"/>
       <c r="E35" s="29" t="s">
-        <v>403</v>
+        <v>384</v>
       </c>
       <c r="F35" s="29"/>
-      <c r="G35" s="34"/>
+      <c r="G35" s="28"/>
       <c r="H35" s="30" t="s">
-        <v>630</v>
-      </c>
-      <c r="I35" s="34"/>
-      <c r="J35" s="34"/>
-      <c r="K35" s="28" t="s">
-        <v>661</v>
-      </c>
-      <c r="L35" s="28" t="s">
-        <v>661</v>
-      </c>
-      <c r="M35" s="28" t="s">
-        <v>661</v>
-      </c>
+        <v>633</v>
+      </c>
+      <c r="I35" s="28"/>
+      <c r="J35" s="28"/>
+      <c r="K35" s="28"/>
+      <c r="L35" s="28"/>
+      <c r="M35" s="28"/>
       <c r="N35" s="28"/>
       <c r="O35" s="33"/>
       <c r="P35" s="33"/>
       <c r="Q35" s="33"/>
       <c r="R35" s="33"/>
-      <c r="S35" s="34"/>
-      <c r="T35" s="34"/>
+      <c r="S35" s="28"/>
+      <c r="T35" s="28"/>
+      <c r="U35" s="7"/>
     </row>
     <row r="36" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B36" s="29" t="s">
-        <v>692</v>
+        <v>658</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>706</v>
+        <v>672</v>
       </c>
       <c r="D36" s="29"/>
       <c r="E36" s="29" t="s">
@@ -4680,14 +4639,20 @@
       <c r="F36" s="29"/>
       <c r="G36" s="34"/>
       <c r="H36" s="30" t="s">
-        <v>673</v>
+        <v>630</v>
       </c>
       <c r="I36" s="34"/>
       <c r="J36" s="34"/>
-      <c r="K36" s="34"/>
-      <c r="L36" s="34"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
+      <c r="K36" s="28" t="s">
+        <v>638</v>
+      </c>
+      <c r="L36" s="28" t="s">
+        <v>638</v>
+      </c>
+      <c r="M36" s="28" t="s">
+        <v>638</v>
+      </c>
+      <c r="N36" s="28"/>
       <c r="O36" s="33"/>
       <c r="P36" s="33"/>
       <c r="Q36" s="33"/>
@@ -4695,55 +4660,54 @@
       <c r="S36" s="34"/>
       <c r="T36" s="34"/>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="C37" s="28"/>
+        <v>658</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>673</v>
+      </c>
       <c r="D37" s="29"/>
       <c r="E37" s="29" t="s">
-        <v>690</v>
+        <v>403</v>
       </c>
       <c r="F37" s="29"/>
-      <c r="G37" s="28"/>
+      <c r="G37" s="34"/>
       <c r="H37" s="30" t="s">
-        <v>639</v>
-      </c>
-      <c r="I37" s="28"/>
-      <c r="J37" s="28"/>
-      <c r="K37" s="28"/>
-      <c r="L37" s="28"/>
-      <c r="M37" s="28"/>
-      <c r="N37" s="28"/>
+        <v>651</v>
+      </c>
+      <c r="I37" s="34"/>
+      <c r="J37" s="34"/>
+      <c r="K37" s="34"/>
+      <c r="L37" s="34"/>
+      <c r="M37" s="34"/>
+      <c r="N37" s="34"/>
       <c r="O37" s="33"/>
       <c r="P37" s="33"/>
       <c r="Q37" s="33"/>
       <c r="R37" s="33"/>
-      <c r="S37" s="28"/>
-      <c r="T37" s="28"/>
-      <c r="U37" s="7"/>
+      <c r="S37" s="34"/>
+      <c r="T37" s="34"/>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C38" s="28" t="s">
-        <v>651</v>
-      </c>
+        <v>659</v>
+      </c>
+      <c r="C38" s="28"/>
       <c r="D38" s="29"/>
       <c r="E38" s="29" t="s">
-        <v>384</v>
+        <v>657</v>
       </c>
       <c r="F38" s="29"/>
       <c r="G38" s="28"/>
       <c r="H38" s="30" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="I38" s="28"/>
       <c r="J38" s="28"/>
@@ -4761,13 +4725,13 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B39" s="29" t="s">
-        <v>692</v>
+        <v>658</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>685</v>
+        <v>702</v>
       </c>
       <c r="D39" s="29"/>
       <c r="E39" s="29" t="s">
@@ -4776,7 +4740,7 @@
       <c r="F39" s="29"/>
       <c r="G39" s="28"/>
       <c r="H39" s="30" t="s">
-        <v>689</v>
+        <v>633</v>
       </c>
       <c r="I39" s="28"/>
       <c r="J39" s="28"/>
@@ -4794,13 +4758,13 @@
     </row>
     <row r="40" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>692</v>
+        <v>658</v>
       </c>
       <c r="C40" s="34" t="s">
-        <v>707</v>
+        <v>674</v>
       </c>
       <c r="D40" s="29"/>
       <c r="E40" s="29" t="s">
@@ -4814,31 +4778,31 @@
       <c r="I40" s="34"/>
       <c r="J40" s="34"/>
       <c r="K40" s="28" t="s">
-        <v>660</v>
+        <v>637</v>
       </c>
       <c r="L40" s="28" t="s">
-        <v>660</v>
+        <v>637</v>
       </c>
       <c r="M40" s="28" t="s">
-        <v>660</v>
+        <v>637</v>
       </c>
       <c r="N40" s="28"/>
-      <c r="O40" s="33"/>
-      <c r="P40" s="33"/>
-      <c r="Q40" s="33"/>
+      <c r="Q40" s="33" t="s">
+        <v>635</v>
+      </c>
       <c r="R40" s="33"/>
       <c r="S40" s="34"/>
       <c r="T40" s="34"/>
     </row>
     <row r="41" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>692</v>
+        <v>658</v>
       </c>
       <c r="C41" s="34" t="s">
-        <v>708</v>
+        <v>675</v>
       </c>
       <c r="D41" s="29"/>
       <c r="E41" s="29" t="s">
@@ -4847,7 +4811,7 @@
       <c r="F41" s="29"/>
       <c r="G41" s="34"/>
       <c r="H41" s="30" t="s">
-        <v>673</v>
+        <v>651</v>
       </c>
       <c r="I41" s="34"/>
       <c r="J41" s="34"/>
@@ -4855,29 +4819,31 @@
       <c r="L41" s="34"/>
       <c r="M41" s="34"/>
       <c r="N41" s="34"/>
-      <c r="O41" s="33"/>
-      <c r="P41" s="33"/>
-      <c r="Q41" s="33"/>
+      <c r="O41" s="35"/>
+      <c r="P41" s="35"/>
+      <c r="Q41" s="33" t="s">
+        <v>636</v>
+      </c>
       <c r="R41" s="33"/>
       <c r="S41" s="34"/>
       <c r="T41" s="34"/>
     </row>
     <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A42" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B42" s="29" t="s">
-        <v>693</v>
+        <v>659</v>
       </c>
       <c r="C42" s="28"/>
       <c r="D42" s="29"/>
       <c r="E42" s="29" t="s">
-        <v>690</v>
+        <v>657</v>
       </c>
       <c r="F42" s="29"/>
       <c r="G42" s="28"/>
       <c r="H42" s="30" t="s">
-        <v>640</v>
+        <v>691</v>
       </c>
       <c r="I42" s="28"/>
       <c r="J42" s="28"/>
@@ -4895,13 +4861,13 @@
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>692</v>
+        <v>658</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>652</v>
+        <v>703</v>
       </c>
       <c r="D43" s="29"/>
       <c r="E43" s="29" t="s">
@@ -4910,7 +4876,7 @@
       <c r="F43" s="29"/>
       <c r="G43" s="28"/>
       <c r="H43" s="30" t="s">
-        <v>688</v>
+        <v>633</v>
       </c>
       <c r="I43" s="28"/>
       <c r="J43" s="28"/>
@@ -4926,48 +4892,53 @@
       <c r="T43" s="28"/>
       <c r="U43" s="7"/>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C44" s="28" t="s">
-        <v>686</v>
+        <v>658</v>
+      </c>
+      <c r="C44" s="34" t="s">
+        <v>679</v>
       </c>
       <c r="D44" s="29"/>
       <c r="E44" s="29" t="s">
-        <v>384</v>
+        <v>403</v>
       </c>
       <c r="F44" s="29"/>
-      <c r="G44" s="28"/>
+      <c r="G44" s="34"/>
       <c r="H44" s="30" t="s">
-        <v>689</v>
-      </c>
-      <c r="I44" s="28"/>
-      <c r="J44" s="28"/>
-      <c r="K44" s="28"/>
-      <c r="L44" s="28"/>
-      <c r="M44" s="28"/>
+        <v>630</v>
+      </c>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="28" t="s">
+        <v>637</v>
+      </c>
+      <c r="L44" s="28" t="s">
+        <v>637</v>
+      </c>
+      <c r="M44" s="28" t="s">
+        <v>637</v>
+      </c>
       <c r="N44" s="28"/>
       <c r="O44" s="33"/>
       <c r="P44" s="33"/>
       <c r="Q44" s="33"/>
       <c r="R44" s="33"/>
-      <c r="S44" s="28"/>
-      <c r="T44" s="28"/>
-      <c r="U44" s="7"/>
+      <c r="S44" s="34"/>
+      <c r="T44" s="34"/>
     </row>
     <row r="45" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>692</v>
+        <v>658</v>
       </c>
       <c r="C45" s="34" t="s">
-        <v>709</v>
+        <v>680</v>
       </c>
       <c r="D45" s="29"/>
       <c r="E45" s="29" t="s">
@@ -4976,77 +4947,70 @@
       <c r="F45" s="29"/>
       <c r="G45" s="34"/>
       <c r="H45" s="30" t="s">
-        <v>630</v>
+        <v>651</v>
       </c>
       <c r="I45" s="34"/>
       <c r="J45" s="34"/>
-      <c r="K45" s="28" t="s">
-        <v>659</v>
-      </c>
-      <c r="L45" s="28" t="s">
-        <v>659</v>
-      </c>
-      <c r="M45" s="28" t="s">
-        <v>659</v>
-      </c>
-      <c r="N45" s="28"/>
-      <c r="Q45" s="33" t="s">
-        <v>657</v>
-      </c>
+      <c r="K45" s="34"/>
+      <c r="L45" s="34"/>
+      <c r="M45" s="34"/>
+      <c r="N45" s="34"/>
+      <c r="O45" s="33"/>
+      <c r="P45" s="33"/>
+      <c r="Q45" s="33"/>
       <c r="R45" s="33"/>
       <c r="S45" s="34"/>
       <c r="T45" s="34"/>
     </row>
-    <row r="46" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C46" s="34" t="s">
-        <v>710</v>
-      </c>
+        <v>659</v>
+      </c>
+      <c r="C46" s="28"/>
       <c r="D46" s="29"/>
       <c r="E46" s="29" t="s">
-        <v>403</v>
+        <v>657</v>
       </c>
       <c r="F46" s="29"/>
-      <c r="G46" s="34"/>
+      <c r="G46" s="28"/>
       <c r="H46" s="30" t="s">
-        <v>673</v>
-      </c>
-      <c r="I46" s="34"/>
-      <c r="J46" s="34"/>
-      <c r="K46" s="34"/>
-      <c r="L46" s="34"/>
-      <c r="M46" s="34"/>
-      <c r="N46" s="34"/>
-      <c r="O46" s="35"/>
-      <c r="P46" s="35"/>
-      <c r="Q46" s="33" t="s">
-        <v>658</v>
-      </c>
+        <v>692</v>
+      </c>
+      <c r="I46" s="28"/>
+      <c r="J46" s="28"/>
+      <c r="K46" s="28"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="28"/>
+      <c r="N46" s="28"/>
+      <c r="O46" s="33"/>
+      <c r="P46" s="33"/>
+      <c r="Q46" s="33"/>
       <c r="R46" s="33"/>
-      <c r="S46" s="34"/>
-      <c r="T46" s="34"/>
+      <c r="S46" s="28"/>
+      <c r="T46" s="28"/>
+      <c r="U46" s="7"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A47" s="28" t="s">
-        <v>643</v>
+        <v>632</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="C47" s="28"/>
+        <v>658</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>704</v>
+      </c>
       <c r="D47" s="29"/>
       <c r="E47" s="29" t="s">
-        <v>690</v>
+        <v>384</v>
       </c>
       <c r="F47" s="29"/>
       <c r="G47" s="28"/>
       <c r="H47" s="30" t="s">
-        <v>641</v>
+        <v>633</v>
       </c>
       <c r="I47" s="28"/>
       <c r="J47" s="28"/>
@@ -5062,308 +5026,75 @@
       <c r="T47" s="28"/>
       <c r="U47" s="7"/>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A48" s="28" t="s">
-        <v>643</v>
+    <row r="48" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>632</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C48" s="28" t="s">
-        <v>653</v>
+        <v>658</v>
+      </c>
+      <c r="C48" s="22" t="s">
+        <v>676</v>
       </c>
       <c r="D48" s="29"/>
-      <c r="E48" s="29" t="s">
-        <v>384</v>
+      <c r="E48" s="26" t="s">
+        <v>403</v>
       </c>
       <c r="F48" s="29"/>
-      <c r="G48" s="28"/>
-      <c r="H48" s="30" t="s">
-        <v>688</v>
-      </c>
-      <c r="I48" s="28"/>
-      <c r="J48" s="28"/>
-      <c r="K48" s="28"/>
-      <c r="L48" s="28"/>
-      <c r="M48" s="28"/>
-      <c r="N48" s="28"/>
-      <c r="O48" s="33"/>
-      <c r="P48" s="33"/>
-      <c r="Q48" s="33"/>
-      <c r="R48" s="33"/>
-      <c r="S48" s="28"/>
-      <c r="T48" s="28"/>
-      <c r="U48" s="7"/>
-    </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
-        <v>643</v>
+      <c r="G48" s="22"/>
+      <c r="H48" s="27" t="s">
+        <v>630</v>
+      </c>
+      <c r="I48" s="22"/>
+      <c r="J48" s="22"/>
+      <c r="K48" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>637</v>
+      </c>
+      <c r="N48" s="3"/>
+      <c r="O48" s="25"/>
+      <c r="P48" s="25"/>
+      <c r="Q48" s="25"/>
+      <c r="R48" s="25"/>
+      <c r="S48" s="22"/>
+      <c r="T48" s="22"/>
+    </row>
+    <row r="49" spans="1:20" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>632</v>
       </c>
       <c r="B49" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C49" s="28" t="s">
-        <v>694</v>
+        <v>658</v>
+      </c>
+      <c r="C49" s="22" t="s">
+        <v>677</v>
       </c>
       <c r="D49" s="29"/>
-      <c r="E49" s="29" t="s">
-        <v>384</v>
+      <c r="E49" s="26" t="s">
+        <v>403</v>
       </c>
       <c r="F49" s="29"/>
-      <c r="G49" s="28"/>
-      <c r="H49" s="30" t="s">
-        <v>689</v>
-      </c>
-      <c r="I49" s="28"/>
-      <c r="J49" s="28"/>
-      <c r="K49" s="28"/>
-      <c r="L49" s="28"/>
-      <c r="M49" s="28"/>
-      <c r="N49" s="28"/>
-      <c r="O49" s="33"/>
-      <c r="P49" s="33"/>
-      <c r="Q49" s="33"/>
-      <c r="R49" s="33"/>
-      <c r="S49" s="28"/>
-      <c r="T49" s="28"/>
-      <c r="U49" s="7"/>
-    </row>
-    <row r="50" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
-        <v>643</v>
-      </c>
-      <c r="B50" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C50" s="34" t="s">
-        <v>714</v>
-      </c>
-      <c r="D50" s="29"/>
-      <c r="E50" s="29" t="s">
-        <v>403</v>
-      </c>
-      <c r="F50" s="29"/>
-      <c r="G50" s="34"/>
-      <c r="H50" s="30" t="s">
-        <v>630</v>
-      </c>
-      <c r="I50" s="34"/>
-      <c r="J50" s="34"/>
-      <c r="K50" s="28" t="s">
-        <v>659</v>
-      </c>
-      <c r="L50" s="28" t="s">
-        <v>659</v>
-      </c>
-      <c r="M50" s="28" t="s">
-        <v>659</v>
-      </c>
-      <c r="N50" s="28"/>
-      <c r="O50" s="33"/>
-      <c r="P50" s="33"/>
-      <c r="Q50" s="33"/>
-      <c r="R50" s="33"/>
-      <c r="S50" s="34"/>
-      <c r="T50" s="34"/>
-    </row>
-    <row r="51" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="28" t="s">
-        <v>643</v>
-      </c>
-      <c r="B51" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C51" s="34" t="s">
-        <v>715</v>
-      </c>
-      <c r="D51" s="29"/>
-      <c r="E51" s="29" t="s">
-        <v>403</v>
-      </c>
-      <c r="F51" s="29"/>
-      <c r="G51" s="34"/>
-      <c r="H51" s="30" t="s">
-        <v>673</v>
-      </c>
-      <c r="I51" s="34"/>
-      <c r="J51" s="34"/>
-      <c r="K51" s="34"/>
-      <c r="L51" s="34"/>
-      <c r="M51" s="34"/>
-      <c r="N51" s="34"/>
-      <c r="O51" s="33"/>
-      <c r="P51" s="33"/>
-      <c r="Q51" s="33"/>
-      <c r="R51" s="33"/>
-      <c r="S51" s="34"/>
-      <c r="T51" s="34"/>
-    </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A52" s="28" t="s">
-        <v>643</v>
-      </c>
-      <c r="B52" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="C52" s="28"/>
-      <c r="D52" s="29"/>
-      <c r="E52" s="29" t="s">
-        <v>690</v>
-      </c>
-      <c r="F52" s="29"/>
-      <c r="G52" s="28"/>
-      <c r="H52" s="30" t="s">
-        <v>642</v>
-      </c>
-      <c r="I52" s="28"/>
-      <c r="J52" s="28"/>
-      <c r="K52" s="28"/>
-      <c r="L52" s="28"/>
-      <c r="M52" s="28"/>
-      <c r="N52" s="28"/>
-      <c r="O52" s="33"/>
-      <c r="P52" s="33"/>
-      <c r="Q52" s="33"/>
-      <c r="R52" s="33"/>
-      <c r="S52" s="28"/>
-      <c r="T52" s="28"/>
-      <c r="U52" s="7"/>
-    </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A53" s="28" t="s">
-        <v>643</v>
-      </c>
-      <c r="B53" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C53" s="28" t="s">
-        <v>654</v>
-      </c>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29" t="s">
-        <v>384</v>
-      </c>
-      <c r="F53" s="29"/>
-      <c r="G53" s="28"/>
-      <c r="H53" s="30" t="s">
-        <v>688</v>
-      </c>
-      <c r="I53" s="28"/>
-      <c r="J53" s="28"/>
-      <c r="K53" s="28"/>
-      <c r="L53" s="28"/>
-      <c r="M53" s="28"/>
-      <c r="N53" s="28"/>
-      <c r="O53" s="33"/>
-      <c r="P53" s="33"/>
-      <c r="Q53" s="33"/>
-      <c r="R53" s="33"/>
-      <c r="S53" s="28"/>
-      <c r="T53" s="28"/>
-      <c r="U53" s="7"/>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A54" s="28" t="s">
-        <v>643</v>
-      </c>
-      <c r="B54" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C54" s="28" t="s">
-        <v>691</v>
-      </c>
-      <c r="D54" s="29"/>
-      <c r="E54" s="29" t="s">
-        <v>384</v>
-      </c>
-      <c r="F54" s="29"/>
-      <c r="G54" s="28"/>
-      <c r="H54" s="30" t="s">
-        <v>689</v>
-      </c>
-      <c r="I54" s="28"/>
-      <c r="J54" s="28"/>
-      <c r="K54" s="28"/>
-      <c r="L54" s="28"/>
-      <c r="M54" s="28"/>
-      <c r="N54" s="28"/>
-      <c r="O54" s="33"/>
-      <c r="P54" s="33"/>
-      <c r="Q54" s="33"/>
-      <c r="R54" s="33"/>
-      <c r="S54" s="28"/>
-      <c r="T54" s="28"/>
-      <c r="U54" s="7"/>
-    </row>
-    <row r="55" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B55" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C55" s="22" t="s">
-        <v>711</v>
-      </c>
-      <c r="D55" s="29"/>
-      <c r="E55" s="26" t="s">
-        <v>403</v>
-      </c>
-      <c r="F55" s="29"/>
-      <c r="G55" s="22"/>
-      <c r="H55" s="27" t="s">
-        <v>630</v>
-      </c>
-      <c r="I55" s="22"/>
-      <c r="J55" s="22"/>
-      <c r="K55" s="3" t="s">
-        <v>659</v>
-      </c>
-      <c r="L55" s="3" t="s">
-        <v>659</v>
-      </c>
-      <c r="M55" s="3" t="s">
-        <v>659</v>
-      </c>
-      <c r="N55" s="3"/>
-      <c r="O55" s="25"/>
-      <c r="P55" s="25"/>
-      <c r="Q55" s="25"/>
-      <c r="R55" s="25"/>
-      <c r="S55" s="22"/>
-      <c r="T55" s="22"/>
-    </row>
-    <row r="56" spans="1:21" s="23" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>643</v>
-      </c>
-      <c r="B56" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="C56" s="22" t="s">
-        <v>712</v>
-      </c>
-      <c r="D56" s="29"/>
-      <c r="E56" s="26" t="s">
-        <v>403</v>
-      </c>
-      <c r="F56" s="29"/>
-      <c r="G56" s="22"/>
-      <c r="H56" s="27" t="s">
-        <v>673</v>
-      </c>
-      <c r="I56" s="22"/>
-      <c r="J56" s="22"/>
-      <c r="K56" s="22"/>
-      <c r="L56" s="22"/>
-      <c r="M56" s="22"/>
-      <c r="N56" s="22"/>
-      <c r="O56" s="25"/>
-      <c r="P56" s="25"/>
-      <c r="Q56" s="25"/>
-      <c r="R56" s="25"/>
-      <c r="S56" s="22"/>
-      <c r="T56" s="22"/>
+      <c r="G49" s="22"/>
+      <c r="H49" s="27" t="s">
+        <v>651</v>
+      </c>
+      <c r="I49" s="22"/>
+      <c r="J49" s="22"/>
+      <c r="K49" s="22"/>
+      <c r="L49" s="22"/>
+      <c r="M49" s="22"/>
+      <c r="N49" s="22"/>
+      <c r="O49" s="25"/>
+      <c r="P49" s="25"/>
+      <c r="Q49" s="25"/>
+      <c r="R49" s="25"/>
+      <c r="S49" s="22"/>
+      <c r="T49" s="22"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -5405,29 +5136,29 @@
           </x14:formula1>
           <xm:sqref>N1:R1</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
+          <x14:formula1>
+            <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>H1</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$B$2:$B$21</xm:f>
           </x14:formula1>
-          <xm:sqref>E57:E1048576</xm:sqref>
+          <xm:sqref>E50:E1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$C$2:$C$15</xm:f>
           </x14:formula1>
-          <xm:sqref>F57:F1048576</xm:sqref>
+          <xm:sqref>F50:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'CV values'!$D$2:$D$60</xm:f>
           </x14:formula1>
           <xm:sqref>G2:G1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>H1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Moved technical note based on QA feedback
</commit_message>
<xml_diff>
--- a/galactose/OLR/OLR_galactose.xlsx
+++ b/galactose/OLR/OLR_galactose.xlsx
@@ -3374,9 +3374,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3551,9 +3551,6 @@
       <c r="N3" s="28"/>
       <c r="O3" s="33"/>
       <c r="P3" s="33"/>
-      <c r="Q3" s="33" t="s">
-        <v>678</v>
-      </c>
       <c r="R3" s="33"/>
       <c r="S3" s="28"/>
       <c r="T3" s="28"/>
@@ -3658,7 +3655,9 @@
       <c r="N6" s="28"/>
       <c r="O6" s="33"/>
       <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
+      <c r="Q6" s="33" t="s">
+        <v>678</v>
+      </c>
       <c r="R6" s="33"/>
       <c r="S6" s="28"/>
       <c r="T6" s="28"/>

</xml_diff>